<commit_message>
Restructured requirement. Added missing requirement and domains
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsavaliya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" tabRatio="876" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" tabRatio="876" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Terminologies used" sheetId="7" state="hidden" r:id="rId1"/>
+    <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
     <sheet name="ItemRegistration" sheetId="8" r:id="rId2"/>
     <sheet name="Subscriber" sheetId="3" r:id="rId3"/>
     <sheet name="BasketSubscription" sheetId="10" r:id="rId4"/>
@@ -24,7 +24,7 @@
     <sheet name="Benefits" sheetId="5" r:id="rId10"/>
     <sheet name="Integration" sheetId="9" r:id="rId11"/>
     <sheet name="Workflows" sheetId="12" r:id="rId12"/>
-    <sheet name="Requirements to be finalize" sheetId="13" state="hidden" r:id="rId13"/>
+    <sheet name="Requirements to be finalize" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -36,15 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="257">
   <si>
     <t>Configure rules for subscription basket</t>
-  </si>
-  <si>
-    <t>User subscription</t>
-  </si>
-  <si>
-    <t>Register a subscriber(different registration schemes?)</t>
   </si>
   <si>
     <t>A subscriber subscribing to a subscriptionable item</t>
@@ -220,16 +214,6 @@
   </si>
   <si>
     <t>Register as a subscriber</t>
-  </si>
-  <si>
-    <t>As a registered user of the shopping application,I will choose the opton to register myself as subscriber so that I can be eligible to subscriber to one or more items for their periodic receipts at my home.</t>
-  </si>
-  <si>
-    <t>optional
-Configurable</t>
-  </si>
-  <si>
-    <t>As a system I may ask registerd user to provide one time registration charges to be paid by him/her to register as a subscriber.</t>
   </si>
   <si>
     <t>Create offer based on Subscription basket</t>
@@ -367,12 +351,6 @@
     <t>As a System I will run basket level validations and display error message in case of any validation fails.</t>
   </si>
   <si>
-    <t>Revise Subscription</t>
-  </si>
-  <si>
-    <t>Add items into subscription basket</t>
-  </si>
-  <si>
     <t xml:space="preserve">As a User  I add a subscription item to a active subscription basket by providing subscryption cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
   </si>
   <si>
@@ -385,9 +363,6 @@
     <t>System routes user to payment system. Payment system send event (success or failure) back to subscription system. Subscription system register revised subscription accordingly.</t>
   </si>
   <si>
-    <t>Unsubscribe items from subscription basket</t>
-  </si>
-  <si>
     <t>As a user I can modify the quantity or number of cycle of one or more subscriptionable items from subscription basket screen.</t>
   </si>
   <si>
@@ -401,9 +376,6 @@
   </si>
   <si>
     <t>As a System I display updated subscription basket.</t>
-  </si>
-  <si>
-    <t>Cancel Subscription</t>
   </si>
   <si>
     <t>User cancel subscription</t>
@@ -876,6 +848,66 @@
   </si>
   <si>
     <t>BASSUB_41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a System I will trigger refund event so that refund domain can consume it to initiate refund </t>
+  </si>
+  <si>
+    <t>BASSUB_42</t>
+  </si>
+  <si>
+    <t>BASSUB_43</t>
+  </si>
+  <si>
+    <t>SUB_01</t>
+  </si>
+  <si>
+    <t>As a Subscriber I fill registration form with required details to register on subscription website.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a System I display registration form with allows subscriber to fill details  (address, contact details like email address, mobile number, alternative contact number). </t>
+  </si>
+  <si>
+    <t>Edit subscriber details</t>
+  </si>
+  <si>
+    <t>As a Subscriber I edit my profile as to keep system updated with my currect contact details.</t>
+  </si>
+  <si>
+    <t>Affiance creates subscriber account with user name as mobile number/email address and allow subscriber to set password.</t>
+  </si>
+  <si>
+    <t>REF_01</t>
+  </si>
+  <si>
+    <t>Register refund event</t>
+  </si>
+  <si>
+    <t>As a System I listen to refund event generated by BasketSubscription as to start refund process</t>
+  </si>
+  <si>
+    <t>Shoipping site will send comfirmation of refund proccess completed in end of the cycle.</t>
+  </si>
+  <si>
+    <t>As a System I will mark  refund process as completed in system.</t>
+  </si>
+  <si>
+    <t>As a System I will communicate refund details to shopping site with details like basketId, subscriberId, refund amount, refund process start date, refund process end date and mark refund process status as 'sent for deposit'.</t>
+  </si>
+  <si>
+    <t>REF_02</t>
+  </si>
+  <si>
+    <t>REF_03</t>
+  </si>
+  <si>
+    <t>REF_04</t>
+  </si>
+  <si>
+    <t>Send refund details to shopping site</t>
+  </si>
+  <si>
+    <t>Mark refund process as complete</t>
   </si>
 </sst>
 </file>
@@ -1317,66 +1349,66 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.35">
@@ -1775,99 +1807,99 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C9" s="3"/>
       <c r="D9" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -1896,98 +1928,98 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1999,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2014,25 +2046,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2040,20 +2072,20 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2061,55 +2093,55 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C12" s="8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="8" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2117,25 +2149,25 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C20" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C21" s="8" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C22" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2161,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2169,7 +2201,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2177,7 +2209,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2185,7 +2217,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2193,7 +2225,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2201,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2213,15 +2245,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7265625" customWidth="1"/>
     <col min="4" max="4" width="53.54296875" customWidth="1"/>
     <col min="5" max="5" width="63.7265625" customWidth="1"/>
     <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
@@ -2230,89 +2262,89 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>107</v>
+        <v>101</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E6" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E8" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E9" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E10" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E11" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2329,180 +2361,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="3"/>
     <col min="2" max="2" width="14.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.26953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="83.7265625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.453125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="3"/>
+    <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>187</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E2" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2"/>
+    </row>
     <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>55</v>
+      <c r="C4" s="1"/>
+      <c r="D4" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="D5" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D18" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D21" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D22" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
@@ -2545,16 +2563,21 @@
       <c r="D30" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
+      <formula1>"Not Started, Completed, In Progress"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2570,544 +2593,561 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>237</v>
+      </c>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>243</v>
+      <c r="A42" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
-        <v>244</v>
+      <c r="A43" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
-        <v>245</v>
+      <c r="A44" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3126,7 +3166,7 @@
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3141,82 +3181,82 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3234,7 +3274,7 @@
   <dimension ref="A2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3249,54 +3289,54 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3314,7 +3354,7 @@
   <dimension ref="A2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3327,42 +3367,42 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3372,14 +3412,185 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="67.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+      <formula1>"Not Started, Completed, In Progress"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3403,101 +3614,101 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addition of pricing requirements and requirements for subscription account
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" tabRatio="876" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="5835" tabRatio="876" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="301">
   <si>
     <t>Configure rules for subscription basket</t>
   </si>
@@ -608,15 +603,6 @@
   </si>
   <si>
     <t>PR_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As an administrtor I will forecast following elements related to a product
-1 Purchase price of the product and change in purchase price during the year
-2. Sale price of a product and change in sale price during the year
-3. Number of new customers subscribed for that product every month 
-4. Number of existing customers left subscription every month
-5. Operationl expense incurred for selling the product.
-6. Sales and Marketing expenses incurred for selling the product. </t>
   </si>
   <si>
     <t>As a system I will use the forcasted attributes by administrator and calculate following metrics
@@ -636,17 +622,6 @@
     <t xml:space="preserve">Read daily values for the attributes for calculating projections </t>
   </si>
   <si>
-    <t xml:space="preserve">As a system I will pick up required data based on acuals for calculating projections for a product based on the the dynamics of the product sale.
-Data Picked up 
-1 Purchase price of the product on a day
-2. Sale price of a product on a day
-3. Number of new customers subscribed for that product on a day 
-4. Number of existing customers left subscription on a day
-5. Operationl expense incurred for selling the product on a day.
-6. Sales and Marketing expenses incurred for selling the product on a day. 
-</t>
-  </si>
-  <si>
     <t>Calculate forecast(projections) based on actual( current and historical) values picked up in earlier user story,using time series analysis.</t>
   </si>
   <si>
@@ -908,6 +883,197 @@
   </si>
   <si>
     <t>Mark refund process as complete</t>
+  </si>
+  <si>
+    <t>As a system I will create a product account for every product that administrator has registered with affaince as a subscriptionable product so as to maintain all product related transactions data in it. It will have following provisions
+1. Forecast
+2. Actuals
+3. Credit points
+4. Total debit
+5. Total Credit
+6.Contingencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create product account </t>
+  </si>
+  <si>
+    <t>As a system I will capture the forecast information under the forecast section of product account When platform administrator creates forecast for a subscriptionable product so as to compare the actual performance of that product against predictions The forecase will have following attributes.
+1. Price bucket containing prediction about changing offering prices/purchase prices
+2. Weight
+3. Profit margin
+4. Categorization
+5. New subscribers per period(week/month)
+6. Churned subscribers per period(week/month) affiliated to each price bucket
+7. From date of forecast
+8. To Date of Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an administrtor I will forecast following elements related to a product
+1 Purchase price of the product and change in purchase price during the year
+2. Sale price of a product and change in sale price during the year
+3. Number of new subscribers subscribed for that product every month 
+4. Number of existing subscribers left subscription every month
+5. Operationl expense incurred for selling the product.
+6. Sales and Marketing expenses incurred for selling the product. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will pick up required data based on acuals for calculating projections for a product based on the the dynamics of the product sale.
+Data Picked up 
+1 Purchase price of the product on a day
+2. Sale price of a product on a day
+3. Number of new subscribers subscribed for that product on a day 
+4. Number of existing subscribers left subscription on a day
+5. Operationl expense incurred for selling the product on a day.
+6. Sales and Marketing expenses incurred for selling the product on a day. 
+</t>
+  </si>
+  <si>
+    <t>Capture forecast for a product</t>
+  </si>
+  <si>
+    <t>Calculate foreasted values of defined metrics for a product</t>
+  </si>
+  <si>
+    <t>Capture Actual values for defined metrics for a product</t>
+  </si>
+  <si>
+    <t>As a System I will calculate the following metrics when subscriber enters forecast details for a product
+1. Monthly operational expenses per product
+2. Monthly sales and marketing expenses per product
+3. Net new subscribers per period(month)
+4. Total subscribers per period(month)
+5. Total churned subscribers per period(month)
+6. Percentage churned subscribers per period(month)
+7.Monthly recurring revenue due to new subscribers( MRR New)
+8. Monthly churned revenue due loosing subscribers associated with each price bucket.
+9. Total Monthly churned revenue
+10. Percentage net revenue churn
+11. Monthly average revenue per subscriber(ARPS New)
+12. Monthly average revenue per total subscribers(ARPS)
+13. Total monthly revenue
+14. Total cost of goods sold
+15. Selling price derived from margin percentage
+16. Operating profit/loss
+17. Percentage operating profit/loss
+18. Subscriber lifetime value(SLV)
+19. Subscriber lifetime period
+20. Cost of acquiring a subscriber(CAS)
+21. SLV to CAS ratio
+22. Months to recover CAS</t>
+  </si>
+  <si>
+    <t>As a System I will update the following attributes in product account for a product when a new subscriber has confirmed subscription,for every product that he/she has subscribed to.
+1. New subscribers associated with current price bucket</t>
+  </si>
+  <si>
+    <t>As a System I will update the following attributes in product account for a product when an existing subscriber has added additional quantity,for that product 
+1. New subscribers associated with current price bucket(not the earlier price bucket where his earlier quantity was registered)</t>
+  </si>
+  <si>
+    <t>As a System I will update the following attributes in product account for a product when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
+1. Churned subscribers associated with current price bucket</t>
+  </si>
+  <si>
+    <t>As a System I will create a new price bucket when offered price of that product (calculated by the system through daily job) changes so that any new subscribers subscribing to that product henceforth can be associated with this price bucket.</t>
+  </si>
+  <si>
+    <t>As a System I will add a new version of a purchase price(COGS) in all available price buckets in the product account of a product when its purchase price undergoes changes (informed by daily feed coming from the main application to subscription platform),so that it can precisely calculate the profits and losses incurred by that product.</t>
+  </si>
+  <si>
+    <t>Compute derived paramteres for a product.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the actual operating expenses per product per month and update it in respective product's product account ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate and credit operating expenses per product per month in the credit attribute Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when customer makes payment for his subscription.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate and debit operating expenses in the debit attribute of Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when a basket is successfully delivered to the customer( as notified by daily feed from main application).</t>
+  </si>
+  <si>
+    <t>Update actual operating expenses credit balance in Operating expenses account</t>
+  </si>
+  <si>
+    <t>Update actual operating expenses debit balance in Operating expenses account.</t>
+  </si>
+  <si>
+    <t>Receive/Compute actual Expense and update in respective product account</t>
+  </si>
+  <si>
+    <t>Forecast operating expenses per product and update in respective product account.</t>
+  </si>
+  <si>
+    <t>Compute actual operating profit per product and update in respective product account</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the computed actual paramters (including operating expenses distribution at daily basis) on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
+  </si>
+  <si>
+    <t>As a system I will calulate the forecasted operating expenses  per product per month  and update it in respective product's product account( forecasted expense attribute for each month) when the administrator confirms/changes the forecast for operating expenses so as to calculate forecasted pricing for that product.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will compute the actual operating profit  per day as a batch job and update(add) it in the operating profit attribute of product account for that day so that at the end of month I can compare it with forecasted operating profit in order to impact pricing of that product as well as contribute/borrow to/from nodal account. </t>
+  </si>
+  <si>
+    <t>Item prices</t>
+  </si>
+  <si>
+    <t>When system activates subscription after receiving payment, as a System I will assign price bucket to each items in the subscription.</t>
+  </si>
+  <si>
+    <t>Item Subscription</t>
+  </si>
+  <si>
+    <t>Basket Activation Event</t>
+  </si>
+  <si>
+    <t>When subscriber increase quantity of perticular item, As a System I will assign new price bucket to newly added quantity.</t>
+  </si>
+  <si>
+    <t>Subscription update accepted event</t>
+  </si>
+  <si>
+    <t>Basket level benefits</t>
+  </si>
+  <si>
+    <t>As a System I will calculate basket level discount based on credit point of basket items, total basket amount, Duration of the subscription, Payment mode, Stability of the basket (no content is changed in the basket after subscription will attract full benefits) when subscriber confirms subscription. Discount can be redemption point, cashback or diect deduction from total amount.</t>
+  </si>
+  <si>
+    <t>Subscription Confirmed event or Subscription update accepted event</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a System I will also provide calculated discount data to item subscription so that It can be shown to subscriber on UI.</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>As a System I will debit (negative) total basket amount for the whole period from subscriber's account when subscribers confirms subscription.</t>
+  </si>
+  <si>
+    <t>Subscription Confirmed event</t>
+  </si>
+  <si>
+    <t>As a System I will credit (possitive) amount in subscriber's account when receives payment from subscription.</t>
+  </si>
+  <si>
+    <t>Payment confirmed event</t>
+  </si>
+  <si>
+    <t>As a System I will send appropriate notifications (email/sms) to subscriber in case of negative amount in the account after due date.</t>
+  </si>
+  <si>
+    <t>Batch operation</t>
+  </si>
+  <si>
+    <t>As a System I will validate that amout is 0 in subscriber's account after delivery of all baskets as to close subscription.</t>
+  </si>
+  <si>
+    <t>Basket</t>
+  </si>
+  <si>
+    <t>Subscription completed event</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1052,6 +1218,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1325,7 +1494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1339,15 +1508,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1796875" style="5"/>
-    <col min="3" max="3" width="17.54296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="102.453125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="5"/>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="17.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="102.42578125" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
         <v>49</v>
       </c>
@@ -1355,7 +1524,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>35</v>
       </c>
@@ -1363,7 +1532,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
@@ -1371,7 +1540,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1379,7 +1548,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
@@ -1387,7 +1556,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C7" s="6" t="s">
         <v>43</v>
       </c>
@@ -1395,7 +1564,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
         <v>44</v>
       </c>
@@ -1403,7 +1572,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="s">
         <v>47</v>
       </c>
@@ -1411,375 +1580,375 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
     </row>
@@ -1797,15 +1966,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7265625" customWidth="1"/>
-    <col min="4" max="4" width="97.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="97.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -1831,7 +2000,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -1843,7 +2012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="144.94999999999999" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -1855,7 +2024,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -1877,7 +2046,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -1896,7 +2065,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
       <c r="C9" s="3"/>
       <c r="D9" s="8" t="s">
         <v>80</v>
@@ -1916,17 +2085,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="5"/>
-    <col min="2" max="2" width="15.7265625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.81640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="37.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="79.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="5"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="15.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="79.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
@@ -1941,7 +2110,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>101</v>
       </c>
@@ -1952,7 +2121,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="159.6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>115</v>
       </c>
@@ -1966,7 +2135,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="116.1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>116</v>
       </c>
@@ -1983,7 +2152,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="144.94999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>118</v>
       </c>
@@ -1997,7 +2166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="101.45" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>122</v>
       </c>
@@ -2008,7 +2177,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>128</v>
       </c>
@@ -2035,13 +2204,13 @@
       <selection activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2052,22 +2221,22 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C3" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2078,17 +2247,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2099,52 +2268,52 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C11" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C12" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C13" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2155,17 +2324,17 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="s">
         <v>165</v>
       </c>
@@ -2183,12 +2352,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.453125" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2196,7 +2365,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2204,7 +2373,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2212,7 +2381,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2220,7 +2389,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2228,7 +2397,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2249,18 +2418,18 @@
       <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7265625" customWidth="1"/>
-    <col min="4" max="4" width="53.54296875" customWidth="1"/>
-    <col min="5" max="5" width="63.7265625" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>103</v>
       </c>
@@ -2275,15 +2444,15 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
         <v>186</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2300,10 +2469,10 @@
         <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="144.94999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -2314,35 +2483,35 @@
         <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="E6" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
       <c r="E8" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E9" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E10" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
         <v>71</v>
       </c>
@@ -2362,26 +2531,26 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
-    <col min="2" max="2" width="14.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="83.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="83.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="3"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -2390,174 +2559,240 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E2" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="8" t="s">
         <v>141</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C8" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C9" s="11"/>
+      <c r="D9" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="11"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="11"/>
+      <c r="D12" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="11"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="11"/>
+      <c r="D15" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="23" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="11"/>
+      <c r="D16" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="23" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="11"/>
+      <c r="D17" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2580,18 +2815,18 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="3"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>100</v>
       </c>
@@ -2605,13 +2840,13 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>108</v>
       </c>
@@ -2622,7 +2857,7 @@
         <v>72</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2633,10 +2868,10 @@
         <v>73</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>110</v>
       </c>
@@ -2644,7 +2879,7 @@
         <v>74</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2658,7 +2893,7 @@
         <v>81</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2672,10 +2907,10 @@
         <v>24</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>113</v>
       </c>
@@ -2684,10 +2919,10 @@
         <v>82</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>114</v>
       </c>
@@ -2696,7 +2931,7 @@
         <v>83</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2709,10 +2944,10 @@
         <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>123</v>
       </c>
@@ -2722,47 +2957,47 @@
         <v>26</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -2770,23 +3005,23 @@
         <v>29</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -2794,23 +3029,23 @@
         <v>30</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -2818,23 +3053,23 @@
         <v>32</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -2842,92 +3077,92 @@
         <v>34</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>155</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
@@ -2937,27 +3172,27 @@
         <v>12</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
@@ -2965,12 +3200,12 @@
         <v>83</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
@@ -2978,12 +3213,12 @@
         <v>86</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
@@ -2991,12 +3226,12 @@
         <v>26</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
@@ -3004,12 +3239,12 @@
         <v>84</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
@@ -3017,12 +3252,12 @@
         <v>87</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
@@ -3030,82 +3265,82 @@
         <v>88</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
         <v>90</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="5" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>94</v>
@@ -3114,40 +3349,40 @@
         <v>95</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>91</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3169,17 +3404,17 @@
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3193,15 +3428,15 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5" t="s">
@@ -3211,12 +3446,12 @@
         <v>18</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
@@ -3226,12 +3461,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
@@ -3241,12 +3476,12 @@
         <v>21</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="5" t="s">
@@ -3256,7 +3491,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3277,17 +3512,17 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.453125" customWidth="1"/>
-    <col min="4" max="4" width="66.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="66.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3301,15 +3536,15 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -3319,12 +3554,12 @@
         <v>121</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>122</v>
@@ -3336,7 +3571,7 @@
         <v>124</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3357,15 +3592,15 @@
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.1796875" customWidth="1"/>
-    <col min="4" max="4" width="52.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3379,13 +3614,13 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
@@ -3393,13 +3628,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
         <v>10</v>
@@ -3418,16 +3653,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="67.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3441,147 +3676,147 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F2" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>251</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>253</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>256</v>
-      </c>
       <c r="D6" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
@@ -3597,22 +3832,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="36.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>100</v>
       </c>
@@ -3626,89 +3861,199 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" ht="188.45" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" ht="159.6" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="57.95" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="375" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>183</v>
+      <c r="C17" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated pricing requirement and changed the domain to product.
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="5835" tabRatio="876" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="876" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <sheet name="Basket" sheetId="14" r:id="rId6"/>
     <sheet name="Notofication" sheetId="16" r:id="rId7"/>
     <sheet name="Refund" sheetId="17" r:id="rId8"/>
-    <sheet name="Pricing" sheetId="11" r:id="rId9"/>
+    <sheet name="product" sheetId="11" r:id="rId9"/>
     <sheet name="Benefits" sheetId="5" r:id="rId10"/>
     <sheet name="Integration" sheetId="9" r:id="rId11"/>
     <sheet name="Workflows" sheetId="12" r:id="rId12"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="341">
   <si>
     <t>Configure rules for subscription basket</t>
   </si>
@@ -596,52 +601,9 @@
     <t>Affiance accourdingly update status and other details in the system.</t>
   </si>
   <si>
-    <t xml:space="preserve">Create monthly forcast for a product for the duration of one year. </t>
-  </si>
-  <si>
-    <t>Calculate  required metrics for evaluation of product performance</t>
-  </si>
-  <si>
     <t>PR_02</t>
   </si>
   <si>
-    <t>As a system I will use the forcasted attributes by administrator and calculate following metrics
-1. Customer churn percentage
-2. Monthly recognized revenue- New
-3..Monthy recognized revenuw - Total
-4. Average revenue per new subscriber
-5. Average revenue per subscriber
-6. Gross margin pecentage
-7. OPerating profit/loass percentage
-8. Subscriber lietime value(SLV)
-9. Cost of acquiring a subscriber(CAS)
-10 SLV/CAS ratio
-11. Period to recover CAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read daily values for the attributes for calculating projections </t>
-  </si>
-  <si>
-    <t>Calculate forecast(projections) based on actual( current and historical) values picked up in earlier user story,using time series analysis.</t>
-  </si>
-  <si>
-    <t>As a system I will use the actual attributes(current and historical)  calculate following metrics for the whole month/year?
-1. Customer churn percentage
-2. Monthly recognized revenue- New
-3..Monthy recognized revenuw - Total
-4. Average revenue per new subscriber
-5. Average revenue per subscriber
-6. Gross margin pecentage
-7. OPerating profit/loass percentage
-8. Subscriber lietime value(SLV)
-9. Cost of acquiring a subscriber(CAS)
-10 SLV/CAS ratio
-11. Period to recover CAS</t>
-  </si>
-  <si>
-    <t>PRI_02</t>
-  </si>
-  <si>
     <t>PR_03</t>
   </si>
   <si>
@@ -664,12 +626,6 @@
   </si>
   <si>
     <t>PR_10</t>
-  </si>
-  <si>
-    <t>?????</t>
-  </si>
-  <si>
-    <t>Compare the projected metrics based on actuals and forecasted metrics and adjust sale price so as to meet the forcast as well as gain required net profit</t>
   </si>
   <si>
     <t>Status</t>
@@ -908,33 +864,7 @@
 8. To Date of Forecast</t>
   </si>
   <si>
-    <t xml:space="preserve">As an administrtor I will forecast following elements related to a product
-1 Purchase price of the product and change in purchase price during the year
-2. Sale price of a product and change in sale price during the year
-3. Number of new subscribers subscribed for that product every month 
-4. Number of existing subscribers left subscription every month
-5. Operationl expense incurred for selling the product.
-6. Sales and Marketing expenses incurred for selling the product. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a system I will pick up required data based on acuals for calculating projections for a product based on the the dynamics of the product sale.
-Data Picked up 
-1 Purchase price of the product on a day
-2. Sale price of a product on a day
-3. Number of new subscribers subscribed for that product on a day 
-4. Number of existing subscribers left subscription on a day
-5. Operationl expense incurred for selling the product on a day.
-6. Sales and Marketing expenses incurred for selling the product on a day. 
-</t>
-  </si>
-  <si>
-    <t>Capture forecast for a product</t>
-  </si>
-  <si>
     <t>Calculate foreasted values of defined metrics for a product</t>
-  </si>
-  <si>
-    <t>Capture Actual values for defined metrics for a product</t>
   </si>
   <si>
     <t>As a System I will calculate the following metrics when subscriber enters forecast details for a product
@@ -970,28 +900,12 @@
 1. New subscribers associated with current price bucket(not the earlier price bucket where his earlier quantity was registered)</t>
   </si>
   <si>
-    <t>As a System I will update the following attributes in product account for a product when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
-1. Churned subscribers associated with current price bucket</t>
-  </si>
-  <si>
     <t>As a System I will create a new price bucket when offered price of that product (calculated by the system through daily job) changes so that any new subscribers subscribing to that product henceforth can be associated with this price bucket.</t>
   </si>
   <si>
     <t>As a System I will add a new version of a purchase price(COGS) in all available price buckets in the product account of a product when its purchase price undergoes changes (informed by daily feed coming from the main application to subscription platform),so that it can precisely calculate the profits and losses incurred by that product.</t>
   </si>
   <si>
-    <t>Compute derived paramteres for a product.</t>
-  </si>
-  <si>
-    <t>As a system I will calculate the actual operating expenses per product per month and update it in respective product's product account ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application.</t>
-  </si>
-  <si>
-    <t>As a system I will calculate and credit operating expenses per product per month in the credit attribute Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when customer makes payment for his subscription.</t>
-  </si>
-  <si>
-    <t>As a system I will calculate and debit operating expenses in the debit attribute of Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when a basket is successfully delivered to the customer( as notified by daily feed from main application).</t>
-  </si>
-  <si>
     <t>Update actual operating expenses credit balance in Operating expenses account</t>
   </si>
   <si>
@@ -1007,9 +921,6 @@
     <t>Compute actual operating profit per product and update in respective product account</t>
   </si>
   <si>
-    <t>As a system I will calculate the computed actual paramters (including operating expenses distribution at daily basis) on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
-  </si>
-  <si>
     <t>As a system I will calulate the forecasted operating expenses  per product per month  and update it in respective product's product account( forecasted expense attribute for each month) when the administrator confirms/changes the forecast for operating expenses so as to calculate forecasted pricing for that product.</t>
   </si>
   <si>
@@ -1074,6 +985,189 @@
   </si>
   <si>
     <t>Subscription completed event</t>
+  </si>
+  <si>
+    <t>Capture forecast for a product(for first time)</t>
+  </si>
+  <si>
+    <t>Replicate actuals of last year as forecast of current year</t>
+  </si>
+  <si>
+    <t>As a System I will replicate actuals of last year in the forecast of current year in an yearly batch job so as to provide default values for the forecast for current year which administrator can modify wherever required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a System I will update the following attributes in product account for a product when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
+1. Churned subscribers associated with specific price bucket(s) </t>
+  </si>
+  <si>
+    <t>Capture Actual values for new customers for a product</t>
+  </si>
+  <si>
+    <t>Capture Actual values for churned customers metrics for a product</t>
+  </si>
+  <si>
+    <t>Capture Actual values for additonal quantity by existing customers for a product</t>
+  </si>
+  <si>
+    <t>Capture Actual values for new price bucket metrics for a product</t>
+  </si>
+  <si>
+    <t>Capture Actual values for changed COGS for a product</t>
+  </si>
+  <si>
+    <t>Receive monthly feed on operating expenses from main application</t>
+  </si>
+  <si>
+    <t>As a system I will receive a file containing details on operating expenses(sbscription dependent expenses ,common expenses) so that the same can be fed to product domain for calculating the price of every product.</t>
+  </si>
+  <si>
+    <t>INT_07</t>
+  </si>
+  <si>
+    <t>PR_11</t>
+  </si>
+  <si>
+    <t>PR_12</t>
+  </si>
+  <si>
+    <t>PR_13</t>
+  </si>
+  <si>
+    <t>PR_14</t>
+  </si>
+  <si>
+    <t>PR_15</t>
+  </si>
+  <si>
+    <t>PR_16</t>
+  </si>
+  <si>
+    <t>PR_17</t>
+  </si>
+  <si>
+    <t>PR_18</t>
+  </si>
+  <si>
+    <t>PR_19</t>
+  </si>
+  <si>
+    <t>PR_20</t>
+  </si>
+  <si>
+    <t>PR_21</t>
+  </si>
+  <si>
+    <t>PR_22</t>
+  </si>
+  <si>
+    <t>PR_23</t>
+  </si>
+  <si>
+    <t>PR_24</t>
+  </si>
+  <si>
+    <t>PR_25</t>
+  </si>
+  <si>
+    <t>PR_26</t>
+  </si>
+  <si>
+    <t>PR_27</t>
+  </si>
+  <si>
+    <t>PR_28</t>
+  </si>
+  <si>
+    <t>PR_29</t>
+  </si>
+  <si>
+    <t>PR_30</t>
+  </si>
+  <si>
+    <t>PR_31</t>
+  </si>
+  <si>
+    <t>PR_32</t>
+  </si>
+  <si>
+    <t>PR_33</t>
+  </si>
+  <si>
+    <t>PR_34</t>
+  </si>
+  <si>
+    <t>PR_35</t>
+  </si>
+  <si>
+    <t>PR_36</t>
+  </si>
+  <si>
+    <t>PR_37</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the actual operating expenses per product per month and update it in respective product's product account ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application so that the actual expenses can contribute to the price determination.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the computed actual parameters (including operating expenses distribution at daily basis) on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
+  </si>
+  <si>
+    <t>Compute derived paramteres for actual values for a product.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate operating expenses per product per month for the number of months for which subscriber has made payment, and add it in the credit expenses attribute  of Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when customer makes payment for his subscription.</t>
+  </si>
+  <si>
+    <t>As a system I will keep the product quantity associated with existing price bucket in case a subscriber reduces the quantity of a product but recalculate his basket level discount so that merchant should get benfitted due to breach of subscription contract by the subscriber.</t>
+  </si>
+  <si>
+    <t>Keep same price bucket for the product quantity reduced by subscriber</t>
+  </si>
+  <si>
+    <t>Feed daily values for the attributes from main application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will receive following attributes of every product and feed it in actuals of respective product account so as to calculate the offered price of a product.
+1 Purchase price of the product on a day
+2. MRP of a product on a day
+3.Current Stock
+</t>
+  </si>
+  <si>
+    <t>PR_01</t>
+  </si>
+  <si>
+    <t>Calculate product price- step1 - Compare revenue</t>
+  </si>
+  <si>
+    <t>As a system I will compare current revenue against the forecasted revenue by means of a daily batch job in order to check if current revenue deviates from forecasted one by threshold percent(configurable. Say 10%) so that price of the product can be altered on this deviation reaching the threshold.</t>
+  </si>
+  <si>
+    <t>As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) so as to check if that product's demand is elastic to variations in price.</t>
+  </si>
+  <si>
+    <t>Calculate product price -step3- Compute demand function</t>
+  </si>
+  <si>
+    <t>Calculate product price-step2- Compute price elasticity of demand and its impact on revenue.</t>
+  </si>
+  <si>
+    <t>As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) as well as its revenue function sso as to check if that product's demand is elastic to variations in price.
+In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.</t>
+  </si>
+  <si>
+    <t>As a system I will compute demand function of a product and determine the values for demand function paramters so that I can predict demand precisely for change in its price.</t>
+  </si>
+  <si>
+    <t>Calculate product price - step 4- Calculate break even price of a product</t>
+  </si>
+  <si>
+    <t>As a system I wil calculate break even price of a product( function of product's purchase prices and all expenses) so that I can validate if the changed price does not become less that break even price.</t>
+  </si>
+  <si>
+    <t>Calculate product price - step 5 Determine revised price of product</t>
+  </si>
+  <si>
+    <t>As a system I will change price of the product based on outcomes of step 1 to 3  and identify the lowest price in current demand curve which is more than break even price  in case the product demand is elasitc for the given price range.</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1126,6 +1220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1157,7 +1257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1221,6 +1321,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1494,7 +1597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1508,15 +1611,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="17.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="102.42578125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.1796875" style="5"/>
+    <col min="3" max="3" width="17.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="102.453125" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
         <v>49</v>
       </c>
@@ -1524,7 +1627,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>35</v>
       </c>
@@ -1532,7 +1635,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
@@ -1540,7 +1643,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1651,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
@@ -1556,7 +1659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="6" t="s">
         <v>43</v>
       </c>
@@ -1564,7 +1667,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
         <v>44</v>
       </c>
@@ -1572,7 +1675,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="s">
         <v>47</v>
       </c>
@@ -1580,375 +1683,375 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
     </row>
@@ -1966,15 +2069,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="97.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7265625" customWidth="1"/>
+    <col min="4" max="4" width="97.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -2000,7 +2103,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -2012,7 +2115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="144.94999999999999" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -2024,7 +2127,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -2046,7 +2149,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2065,7 +2168,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C9" s="3"/>
       <c r="D9" s="8" t="s">
         <v>80</v>
@@ -2079,23 +2182,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A2:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="15.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="79.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.1796875" style="5"/>
+    <col min="2" max="2" width="15.7265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.81640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="79.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
@@ -2110,7 +2213,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>101</v>
       </c>
@@ -2121,7 +2224,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="159.6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>115</v>
       </c>
@@ -2135,7 +2238,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="116.1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>116</v>
       </c>
@@ -2152,7 +2255,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="144.94999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>118</v>
       </c>
@@ -2166,7 +2269,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>122</v>
       </c>
@@ -2177,7 +2280,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>128</v>
       </c>
@@ -2189,6 +2292,20 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2204,13 +2321,13 @@
       <selection activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2221,22 +2338,22 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2247,17 +2364,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2268,52 +2385,52 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C12" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2324,17 +2441,17 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C20" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C21" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C22" s="8" t="s">
         <v>165</v>
       </c>
@@ -2352,12 +2469,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="64.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2365,7 +2482,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2373,7 +2490,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2381,7 +2498,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2389,7 +2506,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2397,7 +2514,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2418,18 +2535,18 @@
       <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7265625" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" customWidth="1"/>
+    <col min="5" max="5" width="63.7265625" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>103</v>
       </c>
@@ -2444,15 +2561,15 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2469,10 +2586,10 @@
         <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="144.94999999999999" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -2483,35 +2600,35 @@
         <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E6" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E8" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E9" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E10" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="E11" s="5" t="s">
         <v>71</v>
       </c>
@@ -2530,27 +2647,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="14.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="83.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="3" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -2559,240 +2676,240 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E2" s="16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="8" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="8" t="s">
         <v>141</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="11" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="11"/>
       <c r="D9" s="23" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="11"/>
       <c r="D10" s="23"/>
       <c r="E10" s="11"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="11" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="11"/>
       <c r="D12" s="23" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="23"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="11"/>
       <c r="D13" s="23"/>
       <c r="E13" s="11"/>
       <c r="F13" s="23"/>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="11"/>
       <c r="D15" s="23" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="23" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="11"/>
       <c r="D16" s="23" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="23" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="11"/>
       <c r="D17" s="23" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2815,18 +2932,18 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>100</v>
       </c>
@@ -2840,13 +2957,13 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>108</v>
       </c>
@@ -2857,7 +2974,7 @@
         <v>72</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2868,10 +2985,10 @@
         <v>73</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>110</v>
       </c>
@@ -2879,7 +2996,7 @@
         <v>74</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2893,7 +3010,7 @@
         <v>81</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2907,10 +3024,10 @@
         <v>24</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="72.599999999999994" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>113</v>
       </c>
@@ -2919,10 +3036,10 @@
         <v>82</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>114</v>
       </c>
@@ -2931,7 +3048,7 @@
         <v>83</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2944,10 +3061,10 @@
         <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>123</v>
       </c>
@@ -2957,47 +3074,47 @@
         <v>26</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -3005,23 +3122,23 @@
         <v>29</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -3029,23 +3146,23 @@
         <v>30</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -3053,23 +3170,23 @@
         <v>32</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3077,92 +3194,92 @@
         <v>34</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>155</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
@@ -3172,27 +3289,27 @@
         <v>12</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
@@ -3200,12 +3317,12 @@
         <v>83</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
@@ -3213,12 +3330,12 @@
         <v>86</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
@@ -3226,12 +3343,12 @@
         <v>26</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
@@ -3239,12 +3356,12 @@
         <v>84</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="57.95" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
@@ -3252,12 +3369,12 @@
         <v>87</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
@@ -3265,82 +3382,82 @@
         <v>88</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
         <v>90</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="5" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>94</v>
@@ -3349,40 +3466,40 @@
         <v>95</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>91</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3404,17 +3521,17 @@
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.26953125" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3428,15 +3545,15 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5" t="s">
@@ -3446,12 +3563,12 @@
         <v>18</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
@@ -3461,12 +3578,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
@@ -3476,12 +3593,12 @@
         <v>21</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="5" t="s">
@@ -3491,7 +3608,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3512,17 +3629,17 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
-    <col min="4" max="4" width="66.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.453125" customWidth="1"/>
+    <col min="4" max="4" width="66.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3536,15 +3653,15 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -3554,12 +3671,12 @@
         <v>121</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="57.95" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>122</v>
@@ -3571,7 +3688,7 @@
         <v>124</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3592,15 +3709,15 @@
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+    <col min="4" max="4" width="52.81640625" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3614,13 +3731,13 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
@@ -3628,13 +3745,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
         <v>10</v>
@@ -3653,16 +3770,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
@@ -3676,147 +3793,147 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="3:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
@@ -3832,22 +3949,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="36.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73.1796875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>100</v>
       </c>
@@ -3861,199 +3978,328 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="C5" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" ht="188.45" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:5" ht="159.6" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="D17" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="1:5" ht="57.95" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="375" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
+        <v>302</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>273</v>
+        <v>330</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>303</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>274</v>
+        <v>334</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>272</v>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="18" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="18" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="18" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged ItemRegistration and Product. Merged Subscriber and BasketSubscription. OLD Sheets not yet deleted.
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -13,9 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
-    <sheet name="ItemRegistration" sheetId="8" r:id="rId2"/>
-    <sheet name="Subscriber" sheetId="3" r:id="rId3"/>
-    <sheet name="BasketSubscription" sheetId="10" r:id="rId4"/>
+    <sheet name="ItemRegistration-OLD" sheetId="8" r:id="rId2"/>
+    <sheet name="Subscriber-OLD" sheetId="3" r:id="rId3"/>
+    <sheet name="Subscriber" sheetId="10" r:id="rId4"/>
     <sheet name="PaymentMode" sheetId="15" r:id="rId5"/>
     <sheet name="Basket" sheetId="14" r:id="rId6"/>
     <sheet name="Notofication" sheetId="16" r:id="rId7"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="378">
   <si>
     <t>Configure rules for subscription basket</t>
   </si>
@@ -127,9 +127,6 @@
 2. Receipt of Payment( before start of Payment span,During payment span)- Before start of span
 2A. Payment percentage: 100%
 THis is how he is configuring the payment to be made for every subscripton cycle in advance.</t>
-  </si>
-  <si>
-    <t>As a system I calculate current price quote for the the subscription item which the user is intending to subscribe and show it as today's offered price,MRP, perentage gain.</t>
   </si>
   <si>
     <t>As a system I will recalculate and show the revised price quotes for each subscription item based on the basket size/amount of basket,supply vs demand statistics of items selected etc.</t>
@@ -339,9 +336,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing subscryption cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
-  </si>
-  <si>
     <t>As a User I keep on adding subscription items to basket by entering subscryption cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles so as to build my subscription basket and finally checkout the basket after finalizing subscription items so as to get the total price to be paid as well as total gain( as compared to total MRP).</t>
   </si>
   <si>
@@ -853,23 +847,249 @@
     <t xml:space="preserve">Create product account </t>
   </si>
   <si>
-    <t>As a system I will capture the forecast information under the forecast section of product account When platform administrator creates forecast for a subscriptionable product so as to compare the actual performance of that product against predictions The forecase will have following attributes.
+    <t>Calculate foreasted values of defined metrics for a product</t>
+  </si>
+  <si>
+    <t>Update actual operating expenses credit balance in Operating expenses account</t>
+  </si>
+  <si>
+    <t>Update actual operating expenses debit balance in Operating expenses account.</t>
+  </si>
+  <si>
+    <t>Item prices</t>
+  </si>
+  <si>
+    <t>When system activates subscription after receiving payment, as a System I will assign price bucket to each items in the subscription.</t>
+  </si>
+  <si>
+    <t>Item Subscription</t>
+  </si>
+  <si>
+    <t>Basket Activation Event</t>
+  </si>
+  <si>
+    <t>When subscriber increase quantity of perticular item, As a System I will assign new price bucket to newly added quantity.</t>
+  </si>
+  <si>
+    <t>Subscription update accepted event</t>
+  </si>
+  <si>
+    <t>Basket level benefits</t>
+  </si>
+  <si>
+    <t>As a System I will calculate basket level discount based on credit point of basket items, total basket amount, Duration of the subscription, Payment mode, Stability of the basket (no content is changed in the basket after subscription will attract full benefits) when subscriber confirms subscription. Discount can be redemption point, cashback or diect deduction from total amount.</t>
+  </si>
+  <si>
+    <t>Subscription Confirmed event or Subscription update accepted event</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a System I will also provide calculated discount data to item subscription so that It can be shown to subscriber on UI.</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>As a System I will debit (negative) total basket amount for the whole period from subscriber's account when subscribers confirms subscription.</t>
+  </si>
+  <si>
+    <t>Subscription Confirmed event</t>
+  </si>
+  <si>
+    <t>As a System I will credit (possitive) amount in subscriber's account when receives payment from subscription.</t>
+  </si>
+  <si>
+    <t>Payment confirmed event</t>
+  </si>
+  <si>
+    <t>As a System I will send appropriate notifications (email/sms) to subscriber in case of negative amount in the account after due date.</t>
+  </si>
+  <si>
+    <t>Batch operation</t>
+  </si>
+  <si>
+    <t>As a System I will validate that amout is 0 in subscriber's account after delivery of all baskets as to close subscription.</t>
+  </si>
+  <si>
+    <t>Basket</t>
+  </si>
+  <si>
+    <t>Subscription completed event</t>
+  </si>
+  <si>
+    <t>Capture forecast for a product(for first time)</t>
+  </si>
+  <si>
+    <t>Replicate actuals of last year as forecast of current year</t>
+  </si>
+  <si>
+    <t>As a System I will replicate actuals of last year in the forecast of current year in an yearly batch job so as to provide default values for the forecast for current year which administrator can modify wherever required.</t>
+  </si>
+  <si>
+    <t>Receive monthly feed on operating expenses from main application</t>
+  </si>
+  <si>
+    <t>As a system I will receive a file containing details on operating expenses(sbscription dependent expenses ,common expenses) so that the same can be fed to product domain for calculating the price of every product.</t>
+  </si>
+  <si>
+    <t>INT_07</t>
+  </si>
+  <si>
+    <t>PR_11</t>
+  </si>
+  <si>
+    <t>PR_12</t>
+  </si>
+  <si>
+    <t>PR_13</t>
+  </si>
+  <si>
+    <t>PR_14</t>
+  </si>
+  <si>
+    <t>PR_15</t>
+  </si>
+  <si>
+    <t>PR_16</t>
+  </si>
+  <si>
+    <t>PR_17</t>
+  </si>
+  <si>
+    <t>PR_18</t>
+  </si>
+  <si>
+    <t>PR_19</t>
+  </si>
+  <si>
+    <t>PR_20</t>
+  </si>
+  <si>
+    <t>PR_21</t>
+  </si>
+  <si>
+    <t>PR_22</t>
+  </si>
+  <si>
+    <t>PR_23</t>
+  </si>
+  <si>
+    <t>PR_24</t>
+  </si>
+  <si>
+    <t>PR_25</t>
+  </si>
+  <si>
+    <t>PR_26</t>
+  </si>
+  <si>
+    <t>PR_28</t>
+  </si>
+  <si>
+    <t>PR_29</t>
+  </si>
+  <si>
+    <t>PR_30</t>
+  </si>
+  <si>
+    <t>PR_31</t>
+  </si>
+  <si>
+    <t>PR_32</t>
+  </si>
+  <si>
+    <t>PR_33</t>
+  </si>
+  <si>
+    <t>PR_34</t>
+  </si>
+  <si>
+    <t>PR_35</t>
+  </si>
+  <si>
+    <t>PR_36</t>
+  </si>
+  <si>
+    <t>PR_37</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the computed actual parameters (including operating expenses distribution at daily basis) on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate operating expenses per product per month for the number of months for which subscriber has made payment, and add it in the credit expenses attribute  of Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when customer makes payment for his subscription.</t>
+  </si>
+  <si>
+    <t>Feed daily values for the attributes from main application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will receive following attributes of every product and feed it in actuals of respective product account so as to calculate the offered price of a product.
+1 Purchase price of the product on a day
+2. MRP of a product on a day
+3.Current Stock
+</t>
+  </si>
+  <si>
+    <t>PR_01</t>
+  </si>
+  <si>
+    <t>Calculate product price- step1 - Compare revenue</t>
+  </si>
+  <si>
+    <t>Capture Actual values for new customers for a product of type "price committed"</t>
+  </si>
+  <si>
+    <t>Capture Actual values for additonal quantity by existing customers for a product of type "price committed"</t>
+  </si>
+  <si>
+    <t>Capture Actual values for churned customers metrics for a product of type "price committed"</t>
+  </si>
+  <si>
+    <t>Keep same price bucket for the product quantity reduced by subscriber for all product types</t>
+  </si>
+  <si>
+    <t>Capture Actual values for new price bucket metrics for a product of type "price committed"</t>
+  </si>
+  <si>
+    <t>Capture Actual values for changed COGS for a product of all types</t>
+  </si>
+  <si>
+    <t>As a System I will add a new version of a purchase price(COGS) in all available price buckets in the product account of a product of all types when its purchase price undergoes changes (informed by daily feed coming from the main application to subscription platform),so that it can precisely calculate the profits and losses incurred by that product.</t>
+  </si>
+  <si>
+    <t>Compute derived paramteres for actual values for a product of any type</t>
+  </si>
+  <si>
+    <t>Forecast operating expenses per product and update in respective product account of product of any type.</t>
+  </si>
+  <si>
+    <t>As a system I will calulate the forecasted operating expenses  per product per month  and update it in respective product's product account of product of any type ( forecasted expense attribute for each month) when the administrator confirms/changes the forecast for operating expenses so as to calculate forecasted pricing for that product.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the actual operating expenses per product per month and update it in respective product's product account of product of any type ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application so that the actual expenses can contribute to the price determination.</t>
+  </si>
+  <si>
+    <t>Receive/Compute actual Expense and update in respective product account of product of any type</t>
+  </si>
+  <si>
+    <t>Define product pricng paramters</t>
+  </si>
+  <si>
+    <t>As a system I will capture the forecast information under the forecast section of product account When platform administrator creates forecast for a subscriptionable product so as to compare the actual performance of that product against predictions The forecast will have following attributes.
 1. Price bucket containing prediction about changing offering prices/purchase prices
 2. Weight
 3. Profit margin
 4. Categorization
 5. New subscribers per period(week/month)
 6. Churned subscribers per period(week/month) affiliated to each price bucket
-7. From date of forecast
-8. To Date of Forecast</t>
-  </si>
-  <si>
-    <t>Calculate foreasted values of defined metrics for a product</t>
+7. List of substitute products ( in case admin has selected "Cross Price Elasitcity" option) 
+8. List of complementory products (in case admin has selected "Cross Price Elasitcity" option)
+9. Advertising expenses per product(in case admin has selected "Advertising expenses" option)
+10. From date of forecast
+11. To Date of Forecast</t>
   </si>
   <si>
     <t>As a System I will calculate the following metrics when subscriber enters forecast details for a product
-1. Monthly operational expenses per product
-2. Monthly sales and marketing expenses per product
+1. Monthly operational expenses per product??
+2. Monthly sales and marketing expenses per product??
 3. Net new subscribers per period(month)
 4. Total subscribers per period(month)
 5. Total churned subscribers per period(month)
@@ -892,282 +1112,199 @@
 22. Months to recover CAS</t>
   </si>
   <si>
-    <t>As a System I will update the following attributes in product account for a product when a new subscriber has confirmed subscription,for every product that he/she has subscribed to.
+    <t>As a System I will add  one(1) in the following attributes in product account for a product of type "price committed" when a new subscriber has confirmed subscription,for every product that he/she has subscribed to.
 1. New subscribers associated with current price bucket</t>
   </si>
   <si>
-    <t>As a System I will update the following attributes in product account for a product when an existing subscriber has added additional quantity,for that product 
+    <t>As a System I will add one(1) in the following attributes in product account for a product  of type "price committed" when an existing subscriber has added additional quantity,for that product 
 1. New subscribers associated with current price bucket(not the earlier price bucket where his earlier quantity was registered)</t>
   </si>
   <si>
-    <t>As a System I will create a new price bucket when offered price of that product (calculated by the system through daily job) changes so that any new subscribers subscribing to that product henceforth can be associated with this price bucket.</t>
-  </si>
-  <si>
-    <t>As a System I will add a new version of a purchase price(COGS) in all available price buckets in the product account of a product when its purchase price undergoes changes (informed by daily feed coming from the main application to subscription platform),so that it can precisely calculate the profits and losses incurred by that product.</t>
-  </si>
-  <si>
-    <t>Update actual operating expenses credit balance in Operating expenses account</t>
-  </si>
-  <si>
-    <t>Update actual operating expenses debit balance in Operating expenses account.</t>
-  </si>
-  <si>
-    <t>Receive/Compute actual Expense and update in respective product account</t>
-  </si>
-  <si>
-    <t>Forecast operating expenses per product and update in respective product account.</t>
-  </si>
-  <si>
-    <t>Compute actual operating profit per product and update in respective product account</t>
-  </si>
-  <si>
-    <t>As a system I will calulate the forecasted operating expenses  per product per month  and update it in respective product's product account( forecasted expense attribute for each month) when the administrator confirms/changes the forecast for operating expenses so as to calculate forecasted pricing for that product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a system I will compute the actual operating profit  per day as a batch job and update(add) it in the operating profit attribute of product account for that day so that at the end of month I can compare it with forecasted operating profit in order to impact pricing of that product as well as contribute/borrow to/from nodal account. </t>
-  </si>
-  <si>
-    <t>Item prices</t>
-  </si>
-  <si>
-    <t>When system activates subscription after receiving payment, as a System I will assign price bucket to each items in the subscription.</t>
-  </si>
-  <si>
-    <t>Item Subscription</t>
-  </si>
-  <si>
-    <t>Basket Activation Event</t>
-  </si>
-  <si>
-    <t>When subscriber increase quantity of perticular item, As a System I will assign new price bucket to newly added quantity.</t>
-  </si>
-  <si>
-    <t>Subscription update accepted event</t>
-  </si>
-  <si>
-    <t>Basket level benefits</t>
-  </si>
-  <si>
-    <t>As a System I will calculate basket level discount based on credit point of basket items, total basket amount, Duration of the subscription, Payment mode, Stability of the basket (no content is changed in the basket after subscription will attract full benefits) when subscriber confirms subscription. Discount can be redemption point, cashback or diect deduction from total amount.</t>
-  </si>
-  <si>
-    <t>Subscription Confirmed event or Subscription update accepted event</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> As a System I will also provide calculated discount data to item subscription so that It can be shown to subscriber on UI.</t>
-  </si>
-  <si>
-    <t>Payments</t>
-  </si>
-  <si>
-    <t>As a System I will debit (negative) total basket amount for the whole period from subscriber's account when subscribers confirms subscription.</t>
-  </si>
-  <si>
-    <t>Subscription Confirmed event</t>
-  </si>
-  <si>
-    <t>As a System I will credit (possitive) amount in subscriber's account when receives payment from subscription.</t>
-  </si>
-  <si>
-    <t>Payment confirmed event</t>
-  </si>
-  <si>
-    <t>As a System I will send appropriate notifications (email/sms) to subscriber in case of negative amount in the account after due date.</t>
-  </si>
-  <si>
-    <t>Batch operation</t>
-  </si>
-  <si>
-    <t>As a System I will validate that amout is 0 in subscriber's account after delivery of all baskets as to close subscription.</t>
-  </si>
-  <si>
-    <t>Basket</t>
-  </si>
-  <si>
-    <t>Subscription completed event</t>
-  </si>
-  <si>
-    <t>Capture forecast for a product(for first time)</t>
-  </si>
-  <si>
-    <t>Replicate actuals of last year as forecast of current year</t>
-  </si>
-  <si>
-    <t>As a System I will replicate actuals of last year in the forecast of current year in an yearly batch job so as to provide default values for the forecast for current year which administrator can modify wherever required.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a System I will update the following attributes in product account for a product when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
+    <t xml:space="preserve">As a System I will add one(1) in the following attributes in product account for a product of type "price committed" when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
 1. Churned subscribers associated with specific price bucket(s) </t>
   </si>
   <si>
-    <t>Capture Actual values for new customers for a product</t>
-  </si>
-  <si>
-    <t>Capture Actual values for churned customers metrics for a product</t>
-  </si>
-  <si>
-    <t>Capture Actual values for additonal quantity by existing customers for a product</t>
-  </si>
-  <si>
-    <t>Capture Actual values for new price bucket metrics for a product</t>
-  </si>
-  <si>
-    <t>Capture Actual values for changed COGS for a product</t>
-  </si>
-  <si>
-    <t>Receive monthly feed on operating expenses from main application</t>
-  </si>
-  <si>
-    <t>As a system I will receive a file containing details on operating expenses(sbscription dependent expenses ,common expenses) so that the same can be fed to product domain for calculating the price of every product.</t>
-  </si>
-  <si>
-    <t>INT_07</t>
-  </si>
-  <si>
-    <t>PR_11</t>
-  </si>
-  <si>
-    <t>PR_12</t>
-  </si>
-  <si>
-    <t>PR_13</t>
-  </si>
-  <si>
-    <t>PR_14</t>
-  </si>
-  <si>
-    <t>PR_15</t>
-  </si>
-  <si>
-    <t>PR_16</t>
-  </si>
-  <si>
-    <t>PR_17</t>
-  </si>
-  <si>
-    <t>PR_18</t>
-  </si>
-  <si>
-    <t>PR_19</t>
-  </si>
-  <si>
-    <t>PR_20</t>
-  </si>
-  <si>
-    <t>PR_21</t>
-  </si>
-  <si>
-    <t>PR_22</t>
-  </si>
-  <si>
-    <t>PR_23</t>
-  </si>
-  <si>
-    <t>PR_24</t>
-  </si>
-  <si>
-    <t>PR_25</t>
-  </si>
-  <si>
-    <t>PR_26</t>
-  </si>
-  <si>
-    <t>PR_27</t>
-  </si>
-  <si>
-    <t>PR_28</t>
-  </si>
-  <si>
-    <t>PR_29</t>
-  </si>
-  <si>
-    <t>PR_30</t>
-  </si>
-  <si>
-    <t>PR_31</t>
-  </si>
-  <si>
-    <t>PR_32</t>
-  </si>
-  <si>
-    <t>PR_33</t>
-  </si>
-  <si>
-    <t>PR_34</t>
-  </si>
-  <si>
-    <t>PR_35</t>
-  </si>
-  <si>
-    <t>PR_36</t>
-  </si>
-  <si>
-    <t>PR_37</t>
-  </si>
-  <si>
-    <t>As a system I will calculate the actual operating expenses per product per month and update it in respective product's product account ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application so that the actual expenses can contribute to the price determination.</t>
-  </si>
-  <si>
-    <t>As a system I will calculate the computed actual parameters (including operating expenses distribution at daily basis) on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
-  </si>
-  <si>
-    <t>Compute derived paramteres for actual values for a product.</t>
-  </si>
-  <si>
-    <t>As a system I will calculate operating expenses per product per month for the number of months for which subscriber has made payment, and add it in the credit expenses attribute  of Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when customer makes payment for his subscription.</t>
-  </si>
-  <si>
-    <t>As a system I will keep the product quantity associated with existing price bucket in case a subscriber reduces the quantity of a product but recalculate his basket level discount so that merchant should get benfitted due to breach of subscription contract by the subscriber.</t>
-  </si>
-  <si>
-    <t>Keep same price bucket for the product quantity reduced by subscriber</t>
-  </si>
-  <si>
-    <t>Feed daily values for the attributes from main application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a system I will receive following attributes of every product and feed it in actuals of respective product account so as to calculate the offered price of a product.
-1 Purchase price of the product on a day
-2. MRP of a product on a day
-3.Current Stock
+    <t>As a system I will reduce the product quantity associated with an existing price bucket in case a subscriber reduces the quantity of a product but recalculate his basket level discount so that merchant should get benfitted due to breach of subscription contract by the subscriber.</t>
+  </si>
+  <si>
+    <t>As a System I will create a new price bucket when offered price of that product of type "price committed" (calculated by the system through daily job) changes so that any new subscribers subscribing to that product henceforth can be associated with this new/latest price bucket.</t>
+  </si>
+  <si>
+    <t>Compute actual revenue per product and update in respective product account of product of any type per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will compute the actual revenue  per day as a batch job and update(add) it in the operating profit attribute of product account for that day so that at the end of day I can compare it with forecasted revenue in order to impact pricing of that product as well as contribute/borrow to/from nodal account. </t>
+  </si>
+  <si>
+    <t>Configuration,product account</t>
+  </si>
+  <si>
+    <t>Integration,Product account</t>
+  </si>
+  <si>
+    <t>product account</t>
+  </si>
+  <si>
+    <t>Yearly/half yearly batch,product account</t>
+  </si>
+  <si>
+    <t>New subscription, product account</t>
+  </si>
+  <si>
+    <t>Added subscripton,product account</t>
+  </si>
+  <si>
+    <t>Cancelled subscription</t>
+  </si>
+  <si>
+    <t>Reduced subscripton quantity,product account</t>
+  </si>
+  <si>
+    <t>Daily pricing batch,product account</t>
+  </si>
+  <si>
+    <t>Integration,product account</t>
+  </si>
+  <si>
+    <t>daily batch,product account</t>
+  </si>
+  <si>
+    <t>Pricing Batch</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an Adminstrator I will define which Parameters shuld be used for detemining the product price so as to decide which data should be captured in product forecast
+1. Demand per price(quantity demanded per unit work period against offered prices) - Manadatory
+   1.1 Demand curve period : 1 month,3 months,6 months, 1year
+    1.2 Price change on X% revenue change/profit change
+2. Cross price Elasticity(optional)
+3. Advertising expenses(optional)
+ </t>
+  </si>
+  <si>
+    <t>As a system I will compare current revenue against the forecasted revenue by means of a daily batch job in order to check if current revenue deviates(increases or decreases) from forecasted one by threshold percent(configurable. Say 10%) so that price of the product can be recalculated on this deviation reaching the threshold.</t>
+  </si>
+  <si>
+    <t>As a system I will compute demand function of a product and determine the values for demand function paramters  using last period( month,3 months etc) demand vs price data so that I can choose  next price( to be change) for which the expected demand will be more than existing  demand.</t>
+  </si>
+  <si>
+    <t>As a system I will form a demand function of the product based on the pricing paramters selected by administrator for that product.
+Example: If admin has only selected price as demand paramter then demand function should get created as 
+Q=a-b*Price
+If admin has selected  cross price elasticity then demand function wil become
+Q=a-b*Price+c*CompPrice-d*SubstPrice
+If admin has also slected effect of advertising xpense the demand function will become
+Q=a-b*Price+c*CompPrice-d*SubstPrice+e*AdvExp</t>
+  </si>
+  <si>
+    <t>Pricing batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) so as to check if that product's demand is elastic to variations in price.
+In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.
+price elasticity of demand(n) = (P/Q)(dQ/dP)
+For price to be reduced price elasticity &lt;-1.( demand is price elastic)
+For price to be increased price elasticity &gt;-1 ( demand is price inelastic)
 </t>
   </si>
   <si>
-    <t>PR_01</t>
-  </si>
-  <si>
-    <t>Calculate product price- step1 - Compare revenue</t>
-  </si>
-  <si>
-    <t>As a system I will compare current revenue against the forecasted revenue by means of a daily batch job in order to check if current revenue deviates from forecasted one by threshold percent(configurable. Say 10%) so that price of the product can be altered on this deviation reaching the threshold.</t>
-  </si>
-  <si>
-    <t>As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) so as to check if that product's demand is elastic to variations in price.</t>
+    <t>As a system I will compute  impact of price elasticity of demand on its revenue so as to determine if change in price will increase or decrease revenue.
+(dTR/dP)/Q=1+ n
+for elastic case where n&lt;-1  (dTR/dP)/Q&lt;0. It means dTR/dP&lt;0(increase in price will reduce TR)
+for inelastic case where n&gt;-1  (dTR/dP)/Q&gt;0. It means dTR/dP&gt;0(increase in price will increase TR) 
+In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.</t>
+  </si>
+  <si>
+    <t>pricing batch</t>
+  </si>
+  <si>
+    <t>As a system I wil calculate break even price of a product( function of product's purchase prices and all expenses) so that I can validate if the changed price does not become less that break even price.
+IS IT REQUIRED.. WHAT IS FORMULA??</t>
+  </si>
+  <si>
+    <t>As a system I will change price of the product based on outcomes of step 1 to 3  and identify the lowest price in current demand curve which is more than break even price as well as satisfy price elasticy rule and revenue effect rule  in case the product demand is elasitc for the given price range.</t>
+  </si>
+  <si>
+    <t>PR_38</t>
+  </si>
+  <si>
+    <t>PR_39</t>
+  </si>
+  <si>
+    <t>PR_40</t>
+  </si>
+  <si>
+    <t>PR_41</t>
+  </si>
+  <si>
+    <t>PR_42</t>
+  </si>
+  <si>
+    <t>PR_43</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Subscriber registration</t>
+  </si>
+  <si>
+    <t>Affiance creates subscriber and subscriber account with user name as mobile number/email address and allow subscriber to set password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing subscription cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
+  </si>
+  <si>
+    <t>Item subcription</t>
+  </si>
+  <si>
+    <t>When system activates subscription after receiving payment, as a System I will assign price bucket to each items in the Subscriber Account.</t>
+  </si>
+  <si>
+    <t>When subscriber increase quantity of perticular item, As a System I will assign new price bucket to newly added quantity and add it in the list against that productID in subscriber account.</t>
+  </si>
+  <si>
+    <t>Calculate product price- step2- Determine demand function</t>
   </si>
   <si>
     <t>Calculate product price -step3- Compute demand function</t>
   </si>
   <si>
-    <t>Calculate product price-step2- Compute price elasticity of demand and its impact on revenue.</t>
-  </si>
-  <si>
-    <t>As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) as well as its revenue function sso as to check if that product's demand is elastic to variations in price.
-In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.</t>
-  </si>
-  <si>
-    <t>As a system I will compute demand function of a product and determine the values for demand function paramters so that I can predict demand precisely for change in its price.</t>
-  </si>
-  <si>
-    <t>Calculate product price - step 4- Calculate break even price of a product</t>
-  </si>
-  <si>
-    <t>As a system I wil calculate break even price of a product( function of product's purchase prices and all expenses) so that I can validate if the changed price does not become less that break even price.</t>
-  </si>
-  <si>
-    <t>Calculate product price - step 5 Determine revised price of product</t>
-  </si>
-  <si>
-    <t>As a system I will change price of the product based on outcomes of step 1 to 3  and identify the lowest price in current demand curve which is more than break even price  in case the product demand is elasitc for the given price range.</t>
+    <t>Calculate product price-step4- Compute price elasticity of demand .</t>
+  </si>
+  <si>
+    <t>Calculate product price-step5- Compute effect of price elasticity of demand  on revenue.</t>
+  </si>
+  <si>
+    <t>Calculate product price - step 6- Calculate break even price of a product</t>
+  </si>
+  <si>
+    <t>Calculate product price - step 7 Determine revised price of product</t>
+  </si>
+  <si>
+    <t>Product -PR22 To PR-29</t>
+  </si>
+  <si>
+    <t>As a system I receive current price quote for a the subscription item from products domain  and show it as today's offered price,MRP, perentage gain so that user can agree to it and confirm his/her subscription to that product.</t>
+  </si>
+  <si>
+    <t>As a System I will run subscription item level validations and display error message in case of any validation fails.
+LIST OF VALIDATIONS ???</t>
+  </si>
+  <si>
+    <t>DUPLICATE OF BASSUB_05??</t>
+  </si>
+  <si>
+    <t>As a System I will calculate basket level discount (only if the minimum threshold amount for the basket is overcome) based on credit point of basket items, total basket amount, Duration of the subscription, Payment mode, Stability of the basket (no content is changed in the basket after subscription will attract full benefits) when subscriber confirms subscription. Discount can be redemption point, cashback or diect deduction from total amount.
+NEED TO DESCRIBE EACH STEP AS SEPERATE USER SOTRY.</t>
+  </si>
+  <si>
+    <t>NOW DUPLICATE</t>
+  </si>
+  <si>
+    <t>BASUB_09</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1324,6 +1461,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1621,66 +1780,66 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.35">
@@ -2079,10 +2238,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -2093,85 +2252,85 @@
     </row>
     <row r="2" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C9" s="3"/>
       <c r="D9" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -2200,10 +2359,10 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
@@ -2215,97 +2374,97 @@
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2332,25 +2491,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2358,20 +2517,20 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2379,55 +2538,55 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C12" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2435,25 +2594,25 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C20" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C21" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C22" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2479,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2487,7 +2646,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2495,7 +2654,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2503,7 +2662,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2511,7 +2670,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2519,7 +2678,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2531,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2548,10 +2707,10 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -2561,76 +2720,79 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A5" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E6" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="E6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E7" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="E7" s="5" t="s">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E8" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="E8" s="5" t="s">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E9" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="E9" s="5" t="s">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E10" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="E10" s="5" t="s">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E11" s="21" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="E11" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2648,7 +2810,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2664,10 +2826,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -2676,10 +2838,10 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -2688,93 +2850,93 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E2" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>177</v>
+      <c r="E3" s="19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="11" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="11"/>
       <c r="D9" s="23" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -2787,23 +2949,23 @@
     <row r="11" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="11" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="11"/>
       <c r="D12" s="23" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="23"/>
@@ -2817,52 +2979,52 @@
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
-      <c r="C14" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>274</v>
+      <c r="C14" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="23" t="s">
-        <v>276</v>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="23" t="s">
-        <v>278</v>
+      <c r="C16" s="30"/>
+      <c r="D16" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="23" t="s">
-        <v>279</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>281</v>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
@@ -2915,7 +3077,7 @@
       <c r="D30" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>"Not Started, Completed, In Progress"</formula1>
     </dataValidation>
@@ -2926,10 +3088,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2938,17 +3100,18 @@
     <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="3"/>
+    <col min="5" max="5" width="19.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
@@ -2956,555 +3119,724 @@
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>175</v>
-      </c>
+      <c r="E1" s="4"/>
       <c r="F1" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="E4" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C7" s="18"/>
+      <c r="D7" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C8" s="18"/>
+      <c r="D8" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="18"/>
+      <c r="D9" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C10" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C12" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="C13" s="26"/>
+      <c r="D13" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+      <c r="A19" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="28" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="1"/>
+      <c r="F21" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>196</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="B22" s="32"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1" t="s">
-        <v>208</v>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B31" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="1"/>
+        <v>195</v>
+      </c>
       <c r="D32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>216</v>
+        <v>198</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="C34" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>221</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B39" s="5"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="22"/>
+      <c r="F44" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="D51" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+      <c r="D54" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>178</v>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F11 F14:F18 F20:F36">
       <formula1>"Not Started, Completed, In Progress"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3533,10 +3865,10 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -3545,15 +3877,15 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5" t="s">
@@ -3563,12 +3895,12 @@
         <v>18</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
@@ -3578,12 +3910,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
@@ -3593,12 +3925,12 @@
         <v>21</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="5" t="s">
@@ -3608,7 +3940,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -3641,10 +3973,10 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -3653,42 +3985,42 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -3719,10 +4051,10 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -3731,10 +4063,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -3781,10 +4113,10 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -3793,64 +4125,64 @@
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>237</v>
-      </c>
       <c r="E3" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>245</v>
-      </c>
       <c r="D6" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3949,27 +4281,28 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E40"/>
+  <dimension ref="A2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.7265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="73.1796875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="12.453125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>13</v>
@@ -3978,328 +4311,453 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="174" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>327</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>328</v>
-      </c>
-      <c r="E5" s="24"/>
-    </row>
-    <row r="6" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>250</v>
+      <c r="B8" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="18" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="18" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="18" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>312</v>
+        <v>292</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
-        <v>320</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="18" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="18" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="18" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="18" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redoing updated requirement and strategies document updated with strategy and requirements for handling operating expenses
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\temp_backup\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="876" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="876" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="351">
   <si>
     <t>Configure rules for subscription basket</t>
   </si>
@@ -544,16 +544,10 @@
     <t>PR_04</t>
   </si>
   <si>
-    <t>PR_05</t>
-  </si>
-  <si>
     <t>PR_06</t>
   </si>
   <si>
     <t>PR_07</t>
-  </si>
-  <si>
-    <t>PR_08</t>
   </si>
   <si>
     <t>PR_09</t>
@@ -844,9 +838,6 @@
     <t>PR_18</t>
   </si>
   <si>
-    <t>PR_19</t>
-  </si>
-  <si>
     <t>PR_20</t>
   </si>
   <si>
@@ -896,9 +887,6 @@
   </si>
   <si>
     <t>PR_37</t>
-  </si>
-  <si>
-    <t>As a system I will calculate the computed actual parameters (including operating expenses distribution at daily basis) on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
   </si>
   <si>
     <t>As a system I will calculate operating expenses per product per month for the number of months for which subscriber has made payment, and add it in the credit expenses attribute  of Operating expenses account (by referring to the latest actual expense per product from respective product accounts,which he has added to his basket) when customer makes payment for his subscription.</t>
@@ -944,23 +932,257 @@
     <t>Compute derived paramteres for actual values for a product of any type</t>
   </si>
   <si>
-    <t>Forecast operating expenses per product and update in respective product account of product of any type.</t>
-  </si>
-  <si>
-    <t>As a system I will calulate the forecasted operating expenses  per product per month  and update it in respective product's product account of product of any type ( forecasted expense attribute for each month) when the administrator confirms/changes the forecast for operating expenses so as to calculate forecasted pricing for that product.</t>
-  </si>
-  <si>
-    <t>As a system I will calculate the actual operating expenses per product per month and update it in respective product's product account of product of any type ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application so that the actual expenses can contribute to the price determination.</t>
-  </si>
-  <si>
-    <t>Receive/Compute actual Expense and update in respective product account of product of any type</t>
-  </si>
-  <si>
-    <t>Define product pricng paramters</t>
-  </si>
-  <si>
-    <t>As a system I will capture the forecast information under the forecast section of product account When platform administrator creates forecast for a subscriptionable product so as to compare the actual performance of that product against predictions The forecast will have following attributes.
-1. Price bucket containing prediction about changing offering prices/purchase prices
+    <t>As a System I will add  one(1) in the following attributes in product account for a product of type "price committed" when a new subscriber has confirmed subscription,for every product that he/she has subscribed to.
+1. New subscribers associated with current price bucket</t>
+  </si>
+  <si>
+    <t>As a System I will add one(1) in the following attributes in product account for a product  of type "price committed" when an existing subscriber has added additional quantity,for that product 
+1. New subscribers associated with current price bucket(not the earlier price bucket where his earlier quantity was registered)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a System I will add one(1) in the following attributes in product account for a product of type "price committed" when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
+1. Churned subscribers associated with specific price bucket(s) </t>
+  </si>
+  <si>
+    <t>As a system I will reduce the product quantity associated with an existing price bucket in case a subscriber reduces the quantity of a product but recalculate his basket level discount so that merchant should get benfitted due to breach of subscription contract by the subscriber.</t>
+  </si>
+  <si>
+    <t>As a System I will create a new price bucket when offered price of that product of type "price committed" (calculated by the system through daily job) changes so that any new subscribers subscribing to that product henceforth can be associated with this new/latest price bucket.</t>
+  </si>
+  <si>
+    <t>Compute actual revenue per product and update in respective product account of product of any type per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will compute the actual revenue  per day as a batch job and update(add) it in the operating profit attribute of product account for that day so that at the end of day I can compare it with forecasted revenue in order to impact pricing of that product as well as contribute/borrow to/from nodal account. </t>
+  </si>
+  <si>
+    <t>Configuration,product account</t>
+  </si>
+  <si>
+    <t>Integration,Product account</t>
+  </si>
+  <si>
+    <t>product account</t>
+  </si>
+  <si>
+    <t>Yearly/half yearly batch,product account</t>
+  </si>
+  <si>
+    <t>New subscription, product account</t>
+  </si>
+  <si>
+    <t>Added subscripton,product account</t>
+  </si>
+  <si>
+    <t>Cancelled subscription</t>
+  </si>
+  <si>
+    <t>Reduced subscripton quantity,product account</t>
+  </si>
+  <si>
+    <t>Daily pricing batch,product account</t>
+  </si>
+  <si>
+    <t>Integration,product account</t>
+  </si>
+  <si>
+    <t>daily batch,product account</t>
+  </si>
+  <si>
+    <t>Pricing Batch</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an Adminstrator I will define which Parameters shuld be used for detemining the product price so as to decide which data should be captured in product forecast
+1. Demand per price(quantity demanded per unit work period against offered prices) - Manadatory
+   1.1 Demand curve period : 1 month,3 months,6 months, 1year
+    1.2 Price change on X% revenue change/profit change
+2. Cross price Elasticity(optional)
+3. Advertising expenses(optional)
+ </t>
+  </si>
+  <si>
+    <t>As a system I will compare current revenue against the forecasted revenue by means of a daily batch job in order to check if current revenue deviates(increases or decreases) from forecasted one by threshold percent(configurable. Say 10%) so that price of the product can be recalculated on this deviation reaching the threshold.</t>
+  </si>
+  <si>
+    <t>As a system I will compute demand function of a product and determine the values for demand function paramters  using last period( month,3 months etc) demand vs price data so that I can choose  next price( to be change) for which the expected demand will be more than existing  demand.</t>
+  </si>
+  <si>
+    <t>As a system I will form a demand function of the product based on the pricing paramters selected by administrator for that product.
+Example: If admin has only selected price as demand paramter then demand function should get created as 
+Q=a-b*Price
+If admin has selected  cross price elasticity then demand function wil become
+Q=a-b*Price+c*CompPrice-d*SubstPrice
+If admin has also slected effect of advertising xpense the demand function will become
+Q=a-b*Price+c*CompPrice-d*SubstPrice+e*AdvExp</t>
+  </si>
+  <si>
+    <t>Pricing batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) so as to check if that product's demand is elastic to variations in price.
+In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.
+price elasticity of demand(n) = (P/Q)(dQ/dP)
+For price to be reduced price elasticity &lt;-1.( demand is price elastic)
+For price to be increased price elasticity &gt;-1 ( demand is price inelastic)
+</t>
+  </si>
+  <si>
+    <t>As a system I will compute  impact of price elasticity of demand on its revenue so as to determine if change in price will increase or decrease revenue.
+(dTR/dP)/Q=1+ n
+for elastic case where n&lt;-1  (dTR/dP)/Q&lt;0. It means dTR/dP&lt;0(increase in price will reduce TR)
+for inelastic case where n&gt;-1  (dTR/dP)/Q&gt;0. It means dTR/dP&gt;0(increase in price will increase TR) 
+In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.</t>
+  </si>
+  <si>
+    <t>pricing batch</t>
+  </si>
+  <si>
+    <t>As a system I wil calculate break even price of a product( function of product's purchase prices and all expenses) so that I can validate if the changed price does not become less that break even price.
+IS IT REQUIRED.. WHAT IS FORMULA??</t>
+  </si>
+  <si>
+    <t>As a system I will change price of the product based on outcomes of step 1 to 3  and identify the lowest price in current demand curve which is more than break even price as well as satisfy price elasticy rule and revenue effect rule  in case the product demand is elasitc for the given price range.</t>
+  </si>
+  <si>
+    <t>PR_38</t>
+  </si>
+  <si>
+    <t>PR_39</t>
+  </si>
+  <si>
+    <t>PR_40</t>
+  </si>
+  <si>
+    <t>PR_41</t>
+  </si>
+  <si>
+    <t>PR_42</t>
+  </si>
+  <si>
+    <t>PR_43</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Subscriber registration</t>
+  </si>
+  <si>
+    <t>Affiance creates subscriber and subscriber account with user name as mobile number/email address and allow subscriber to set password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing subscription cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
+  </si>
+  <si>
+    <t>Item subcription</t>
+  </si>
+  <si>
+    <t>When system activates subscription after receiving payment, as a System I will assign price bucket to each items in the Subscriber Account.</t>
+  </si>
+  <si>
+    <t>When subscriber increase quantity of perticular item, As a System I will assign new price bucket to newly added quantity and add it in the list against that productID in subscriber account.</t>
+  </si>
+  <si>
+    <t>Calculate product price- step2- Determine demand function</t>
+  </si>
+  <si>
+    <t>Calculate product price -step3- Compute demand function</t>
+  </si>
+  <si>
+    <t>Calculate product price-step4- Compute price elasticity of demand .</t>
+  </si>
+  <si>
+    <t>Calculate product price-step5- Compute effect of price elasticity of demand  on revenue.</t>
+  </si>
+  <si>
+    <t>Calculate product price - step 6- Calculate break even price of a product</t>
+  </si>
+  <si>
+    <t>Calculate product price - step 7 Determine revised price of product</t>
+  </si>
+  <si>
+    <t>Product -PR22 To PR-29</t>
+  </si>
+  <si>
+    <t>As a system I receive current price quote for a the subscription item from products domain  and show it as today's offered price,MRP, perentage gain so that user can agree to it and confirm his/her subscription to that product.</t>
+  </si>
+  <si>
+    <t>As a System I will run subscription item level validations and display error message in case of any validation fails.
+LIST OF VALIDATIONS ???</t>
+  </si>
+  <si>
+    <t>DUPLICATE OF BASSUB_05??</t>
+  </si>
+  <si>
+    <t>As a System I will calculate basket level discount (only if the minimum threshold amount for the basket is overcome) based on credit point of basket items, total basket amount, Duration of the subscription, Payment mode, Stability of the basket (no content is changed in the basket after subscription will attract full benefits) when subscriber confirms subscription. Discount can be redemption point, cashback or diect deduction from total amount.
+NEED TO DESCRIBE EACH STEP AS SEPERATE USER SOTRY.</t>
+  </si>
+  <si>
+    <t>NOW DUPLICATE</t>
+  </si>
+  <si>
+    <t>BASUB_09</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>PostConfiguration</t>
+  </si>
+  <si>
+    <t>Define product pricing paramters</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>pricing</t>
+  </si>
+  <si>
+    <t>Auto configuration</t>
+  </si>
+  <si>
+    <t>post configuration</t>
+  </si>
+  <si>
+    <t>As a system I will calculate the computed actual parameters on a daily basis by means of a batch job so as to determine the impact of new subscriptions,additions and churning on the performance of the product. This batch should run before the pricing determination batch job.</t>
+  </si>
+  <si>
+    <t>operating expenses</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>Capture operating expenses forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an administrator I will add following paramters so as to calculate forecasted/actual operating expenses
+1. Common expenses
+     -New- Software maintenance and enhancement cost = X Rs per Year
+     -New - Expenses on communication charges(telephoe bill/internet) = Y Rs per month/year
+     -New  - Electricity charges - Z Rs per month/year
+     -New -  Rental expenses - A Rs per month/year
+     -New -  Personnel related expenses(salary,bonus etc) - B Rs per month/year
+     -New -  Taxes/service charges - C Rs per month/year
+     -New -  Housekeeping expenses - D Rs per month/year
+     -New - Cost of recurring travel - E Rs per month/year 
+     -New - printing/stationary charges  - F Rs per month/year 
+     - New- Renewals of licenses/permits/certifications - G Rs per year
+2.Subscripton specific expense 
+New - delivery expenses per weight -
+                 -New - delivery cost from 0 kg to 1 kg = X Rs
+                 -New - delivery cost from 1 kg to 2 kg = Y Rs
+                 -New - deivery cost from 2 kg to 3 kg = Z Rs
+                 -New - deivery cost from 3 kg to 5 kg = A Rs
+  </t>
+  </si>
+  <si>
+    <t>As an administrator I create forecast for a subscriptionable product so as to compare the actual performance of that product against predictions. The structure(for every product) will have following attributes.
+1. Price buckets containing prediction about changing offering prices/purchase prices
 2. Weight
 3. Profit margin
 4. Categorization
@@ -974,7 +1196,7 @@
   </si>
   <si>
     <t>As a System I will calculate the following metrics when subscriber enters forecast details for a product
-1. Monthly operational expenses per product??
+1. Monthly operating expenses per product( sum of commong expenses and subscription specific expenses)
 2. Monthly sales and marketing expenses per product??
 3. Net new subscribers per period(month)
 4. Total subscribers per period(month)
@@ -998,199 +1220,28 @@
 22. Months to recover CAS</t>
   </si>
   <si>
-    <t>As a System I will add  one(1) in the following attributes in product account for a product of type "price committed" when a new subscriber has confirmed subscription,for every product that he/she has subscribed to.
-1. New subscribers associated with current price bucket</t>
-  </si>
-  <si>
-    <t>As a System I will add one(1) in the following attributes in product account for a product  of type "price committed" when an existing subscriber has added additional quantity,for that product 
-1. New subscribers associated with current price bucket(not the earlier price bucket where his earlier quantity was registered)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a System I will add one(1) in the following attributes in product account for a product of type "price committed" when an existing subscriber(associated with a specific price bucket) has cancelled subscription for that product.
-1. Churned subscribers associated with specific price bucket(s) </t>
-  </si>
-  <si>
-    <t>As a system I will reduce the product quantity associated with an existing price bucket in case a subscriber reduces the quantity of a product but recalculate his basket level discount so that merchant should get benfitted due to breach of subscription contract by the subscriber.</t>
-  </si>
-  <si>
-    <t>As a System I will create a new price bucket when offered price of that product of type "price committed" (calculated by the system through daily job) changes so that any new subscribers subscribing to that product henceforth can be associated with this new/latest price bucket.</t>
-  </si>
-  <si>
-    <t>Compute actual revenue per product and update in respective product account of product of any type per day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a system I will compute the actual revenue  per day as a batch job and update(add) it in the operating profit attribute of product account for that day so that at the end of day I can compare it with forecasted revenue in order to impact pricing of that product as well as contribute/borrow to/from nodal account. </t>
-  </si>
-  <si>
-    <t>Configuration,product account</t>
-  </si>
-  <si>
-    <t>Integration,Product account</t>
-  </si>
-  <si>
-    <t>product account</t>
-  </si>
-  <si>
-    <t>Yearly/half yearly batch,product account</t>
-  </si>
-  <si>
-    <t>New subscription, product account</t>
-  </si>
-  <si>
-    <t>Added subscripton,product account</t>
-  </si>
-  <si>
-    <t>Cancelled subscription</t>
-  </si>
-  <si>
-    <t>Reduced subscripton quantity,product account</t>
-  </si>
-  <si>
-    <t>Daily pricing batch,product account</t>
-  </si>
-  <si>
-    <t>Integration,product account</t>
-  </si>
-  <si>
-    <t>daily batch,product account</t>
-  </si>
-  <si>
-    <t>Pricing Batch</t>
-  </si>
-  <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As an Adminstrator I will define which Parameters shuld be used for detemining the product price so as to decide which data should be captured in product forecast
-1. Demand per price(quantity demanded per unit work period against offered prices) - Manadatory
-   1.1 Demand curve period : 1 month,3 months,6 months, 1year
-    1.2 Price change on X% revenue change/profit change
-2. Cross price Elasticity(optional)
-3. Advertising expenses(optional)
- </t>
-  </si>
-  <si>
-    <t>As a system I will compare current revenue against the forecasted revenue by means of a daily batch job in order to check if current revenue deviates(increases or decreases) from forecasted one by threshold percent(configurable. Say 10%) so that price of the product can be recalculated on this deviation reaching the threshold.</t>
-  </si>
-  <si>
-    <t>As a system I will compute demand function of a product and determine the values for demand function paramters  using last period( month,3 months etc) demand vs price data so that I can choose  next price( to be change) for which the expected demand will be more than existing  demand.</t>
-  </si>
-  <si>
-    <t>As a system I will form a demand function of the product based on the pricing paramters selected by administrator for that product.
-Example: If admin has only selected price as demand paramter then demand function should get created as 
-Q=a-b*Price
-If admin has selected  cross price elasticity then demand function wil become
-Q=a-b*Price+c*CompPrice-d*SubstPrice
-If admin has also slected effect of advertising xpense the demand function will become
-Q=a-b*Price+c*CompPrice-d*SubstPrice+e*AdvExp</t>
-  </si>
-  <si>
-    <t>Pricing batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a system I will compute price elasticity of demand for a product for latest period( 1 month,3 months etc.) so as to check if that product's demand is elastic to variations in price.
-In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.
-price elasticity of demand(n) = (P/Q)(dQ/dP)
-For price to be reduced price elasticity &lt;-1.( demand is price elastic)
-For price to be increased price elasticity &gt;-1 ( demand is price inelastic)
+    <t>Calculate operating expenses per product and update in respective product account of product of any type.</t>
+  </si>
+  <si>
+    <t>As a system I will update the calculated actual operating expenses per product per item per month  in respective product's product account of product of any type ( actual expenses attribute) when platform receives monthly feed on operating expenses from main application so that the actual expenses can contribute to the price determination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A system will calculate operating expenses to be incurred by a product per unit as a monthly job when I receive the mothly feed on operating expenses from main application,so that they can be accounted in determining the breakeven price of product.
+1. All expneses listed under common expenses will be interpolated at monthly level ,summed up to form total common expenses and equally distributed among all items subscribed so far from all subscriptionable product. From this every product's share of total common expenses is seprated out(based on total items subscribed for that product), and per unit commong expenses for a product are calculated.
+2.  All expenses listed under subscripton specific expenses(currently only delivery expenses are calculated in the followiing way.
+2.1. Get the list of all delivery rates for every weight range (20 Rs. up to 1s kg, 25 Rs for goods from 1 to 2 kg etc.).
+2.2. Get monthly baskets fitting into each weight range. In case of weekly baskets multiply each by two. In case of quarterly basket divide total baskets by 3 to arrive at total monthly baskets).
+2.3. Apply appropriate delivery rate for baskets in each weigh range and find out total delivery cost to be paid for delivering basket in each weight range per month.
+2.4. Now get items of each subscriptionable product associated with number of baskets falling under each weight range. Same product may be contained in baskets falling under different weight ranges. 
+2.5 Since each product has its weight registered with it, multiply  unit product weight with number of products(contained in baskets with specific weight range) so as to calculate total weight getting delivered under each weight range. 
+2.6 Multiple per kg delivery cost to this total weight (in kgs) to calculate how much delivery cost a product is bearing under each weight range. For the same product calculate it for all weight ranges.
+2.7. Calculate the total delivery (per month) is to be borne by a product, by summing up the costs calculated for each weight range in step 2.4.
+2.8. Repeat this for all products contained in baskets falling under different weight ranges.
+2.9. Total sum of monthly delivery cost for each product should match the cost found at basket level in step 2.3.
 </t>
   </si>
   <si>
-    <t>As a system I will compute  impact of price elasticity of demand on its revenue so as to determine if change in price will increase or decrease revenue.
-(dTR/dP)/Q=1+ n
-for elastic case where n&lt;-1  (dTR/dP)/Q&lt;0. It means dTR/dP&lt;0(increase in price will reduce TR)
-for inelastic case where n&gt;-1  (dTR/dP)/Q&gt;0. It means dTR/dP&gt;0(increase in price will increase TR) 
-In case of elasitc products price reduction increases overall revenue but in case of inelastic products it will result in ultimate reduction of revenue.</t>
-  </si>
-  <si>
-    <t>pricing batch</t>
-  </si>
-  <si>
-    <t>As a system I wil calculate break even price of a product( function of product's purchase prices and all expenses) so that I can validate if the changed price does not become less that break even price.
-IS IT REQUIRED.. WHAT IS FORMULA??</t>
-  </si>
-  <si>
-    <t>As a system I will change price of the product based on outcomes of step 1 to 3  and identify the lowest price in current demand curve which is more than break even price as well as satisfy price elasticy rule and revenue effect rule  in case the product demand is elasitc for the given price range.</t>
-  </si>
-  <si>
-    <t>PR_38</t>
-  </si>
-  <si>
-    <t>PR_39</t>
-  </si>
-  <si>
-    <t>PR_40</t>
-  </si>
-  <si>
-    <t>PR_41</t>
-  </si>
-  <si>
-    <t>PR_42</t>
-  </si>
-  <si>
-    <t>PR_43</t>
-  </si>
-  <si>
-    <t>Configuration</t>
-  </si>
-  <si>
-    <t>Subscriber registration</t>
-  </si>
-  <si>
-    <t>Affiance creates subscriber and subscriber account with user name as mobile number/email address and allow subscriber to set password.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing subscription cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
-  </si>
-  <si>
-    <t>Item subcription</t>
-  </si>
-  <si>
-    <t>When system activates subscription after receiving payment, as a System I will assign price bucket to each items in the Subscriber Account.</t>
-  </si>
-  <si>
-    <t>When subscriber increase quantity of perticular item, As a System I will assign new price bucket to newly added quantity and add it in the list against that productID in subscriber account.</t>
-  </si>
-  <si>
-    <t>Calculate product price- step2- Determine demand function</t>
-  </si>
-  <si>
-    <t>Calculate product price -step3- Compute demand function</t>
-  </si>
-  <si>
-    <t>Calculate product price-step4- Compute price elasticity of demand .</t>
-  </si>
-  <si>
-    <t>Calculate product price-step5- Compute effect of price elasticity of demand  on revenue.</t>
-  </si>
-  <si>
-    <t>Calculate product price - step 6- Calculate break even price of a product</t>
-  </si>
-  <si>
-    <t>Calculate product price - step 7 Determine revised price of product</t>
-  </si>
-  <si>
-    <t>Product -PR22 To PR-29</t>
-  </si>
-  <si>
-    <t>As a system I receive current price quote for a the subscription item from products domain  and show it as today's offered price,MRP, perentage gain so that user can agree to it and confirm his/her subscription to that product.</t>
-  </si>
-  <si>
-    <t>As a System I will run subscription item level validations and display error message in case of any validation fails.
-LIST OF VALIDATIONS ???</t>
-  </si>
-  <si>
-    <t>DUPLICATE OF BASSUB_05??</t>
-  </si>
-  <si>
-    <t>As a System I will calculate basket level discount (only if the minimum threshold amount for the basket is overcome) based on credit point of basket items, total basket amount, Duration of the subscription, Payment mode, Stability of the basket (no content is changed in the basket after subscription will attract full benefits) when subscriber confirms subscription. Discount can be redemption point, cashback or diect deduction from total amount.
-NEED TO DESCRIBE EACH STEP AS SEPERATE USER SOTRY.</t>
-  </si>
-  <si>
-    <t>NOW DUPLICATE</t>
-  </si>
-  <si>
-    <t>BASUB_09</t>
+    <t>Update actual Expense in respective product account of product of any type</t>
   </si>
 </sst>
 </file>
@@ -2095,7 +2146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A57" sqref="A57:F60"/>
     </sheetView>
   </sheetViews>
@@ -2126,10 +2177,10 @@
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2143,10 +2194,10 @@
         <v>65</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2157,10 +2208,10 @@
         <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2171,10 +2222,10 @@
         <v>67</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2182,37 +2233,37 @@
         <v>51</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="16"/>
       <c r="D7" s="22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C8" s="16"/>
       <c r="D8" s="22" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2222,19 +2273,19 @@
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2245,39 +2296,39 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C12" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>229</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="C13" s="23"/>
       <c r="D13" s="24" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="E13" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>230</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2291,17 +2342,17 @@
         <v>100</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -2314,7 +2365,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2323,11 +2374,11 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -2335,7 +2386,7 @@
         <v>107</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16" t="s">
@@ -2343,25 +2394,25 @@
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -2369,7 +2420,7 @@
         <v>111</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20" t="s">
@@ -2377,12 +2428,12 @@
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
@@ -2390,12 +2441,12 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="1"/>
@@ -2404,24 +2455,24 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2430,24 +2481,24 @@
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2456,24 +2507,24 @@
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2482,24 +2533,24 @@
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2508,12 +2559,12 @@
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
@@ -2521,85 +2572,85 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>137</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="1" t="s">
@@ -2610,28 +2661,28 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="1"/>
@@ -2640,12 +2691,12 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="1"/>
@@ -2654,12 +2705,12 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="1"/>
@@ -2668,12 +2719,12 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="1"/>
@@ -2682,12 +2733,12 @@
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="1"/>
@@ -2696,12 +2747,12 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="20"/>
@@ -2710,27 +2761,27 @@
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
@@ -2738,12 +2789,12 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="4" t="s">
@@ -2751,12 +2802,12 @@
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
@@ -2764,33 +2815,33 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>86</v>
@@ -2800,48 +2851,48 @@
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>83</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>108</v>
@@ -2850,12 +2901,12 @@
         <v>109</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>110</v>
@@ -2867,68 +2918,68 @@
         <v>112</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B57"/>
       <c r="C57" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F57"/>
     </row>
     <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B58"/>
       <c r="C58" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F58"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B59"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F59"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B60"/>
       <c r="C60" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F60"/>
     </row>
@@ -2973,10 +3024,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -3006,483 +3057,563 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E46"/>
+  <dimension ref="A2:F44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="73.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>225</v>
+        <v>334</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
+      <c r="C8" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="377" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E7" s="1" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E13" s="1" t="s">
+    <row r="25" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E16" s="1" t="s">
+    <row r="27" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E19" s="1" t="s">
+    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>282</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F29" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="145" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="145" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
+      <c r="F30" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="16" t="s">
         <v>257</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="16" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -3726,16 +3857,16 @@
     </row>
     <row r="10" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3923,15 +4054,15 @@
         <v>14</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
@@ -3941,12 +4072,12 @@
         <v>18</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4" t="s">
@@ -3956,12 +4087,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
@@ -3971,12 +4102,12 @@
         <v>21</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -3986,7 +4117,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added traceability for Subscriber requirements
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\temp_backup\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="876" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5700" tabRatio="876" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="367">
   <si>
     <t>Configure rules for subscription basket</t>
   </si>
@@ -782,12 +782,6 @@
   </si>
   <si>
     <t>Item Subscription</t>
-  </si>
-  <si>
-    <t>Basket Activation Event</t>
-  </si>
-  <si>
-    <t>Subscription update accepted event</t>
   </si>
   <si>
     <t>Basket level benefits</t>
@@ -1243,12 +1237,68 @@
   <si>
     <t>Update actual Expense in respective product account of product of any type</t>
   </si>
+  <si>
+    <t>REST</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Aggregate</t>
+  </si>
+  <si>
+    <t>CommandHandler</t>
+  </si>
+  <si>
+    <t>Event Handler</t>
+  </si>
+  <si>
+    <t>Event Listeners</t>
+  </si>
+  <si>
+    <t>Exception handling</t>
+  </si>
+  <si>
+    <t>BasketRulesController -&gt;addBasketRules, updateBasketRules</t>
+  </si>
+  <si>
+    <t>AddBasketRulesCommand</t>
+  </si>
+  <si>
+    <t>SubscriberController-&gt;createSubscriber</t>
+  </si>
+  <si>
+    <t>CreateSubscriberCommand</t>
+  </si>
+  <si>
+    <t>SubscriberController-&gt;createPassword</t>
+  </si>
+  <si>
+    <t>SetSubscriberPasswordCommand</t>
+  </si>
+  <si>
+    <t>SubscriberController-&gt;updateSubscriberContactDetails
+SubscriberController-&gt;updateSubscriberAddress</t>
+  </si>
+  <si>
+    <t>UpdateSubscriberContactDetailsCommand
+UpdateSubscriberAddressCommand</t>
+  </si>
+  <si>
+    <t>SubscriptionController-&gt;addItemToConsumerBasket</t>
+  </si>
+  <si>
+    <t>AddItemToSubscriptionCommand</t>
+  </si>
+  <si>
+    <t>PRODUCT-&gt;PRICING domain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1273,6 +1323,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1331,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1374,37 +1439,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1689,7 +1772,7 @@
   <dimension ref="C2:D102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2144,844 +2227,885 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:F60"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.26953125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="9.7265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="21"/>
+    <col min="4" max="4" width="75.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="16.26953125" style="21"/>
+    <col min="8" max="8" width="19.453125" style="21" customWidth="1"/>
+    <col min="9" max="16384" width="16.26953125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="29" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="H1" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="39" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="39" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="39" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="26" x14ac:dyDescent="0.3">
+      <c r="C6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="26" x14ac:dyDescent="0.3">
+      <c r="C7" s="18"/>
+      <c r="D7" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="26" x14ac:dyDescent="0.3">
+      <c r="C8" s="18"/>
+      <c r="D8" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="E8" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="78" x14ac:dyDescent="0.3">
+      <c r="C10" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="30" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="H10" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="52" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="H11" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="26" x14ac:dyDescent="0.3">
+      <c r="C12" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="39" x14ac:dyDescent="0.3">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:13" ht="78" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="C6" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="F6" s="17" t="s">
+    <row r="16" spans="1:13" ht="65" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="16"/>
-      <c r="D7" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="F7" s="17" t="s">
+    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="30" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="C8" s="16"/>
-      <c r="D8" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="F8" s="17" t="s">
+    <row r="19" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="26" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="25" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="16"/>
-      <c r="D9" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
+    <row r="22" spans="1:6" ht="52" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="91" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="25" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="C10" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
+    <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A34" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="39" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A37" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A38" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A39" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="17"/>
+      <c r="F39" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A40" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A41" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A42" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="17"/>
+      <c r="F42" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+      <c r="A43" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="17"/>
+      <c r="F43" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A44" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44" s="26"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="23"/>
+      <c r="F44" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A45" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="17"/>
+      <c r="F45" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A46" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="17"/>
+      <c r="F46" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A47" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C47" s="17"/>
+      <c r="D47" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="F48" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A51" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A52" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="65" x14ac:dyDescent="0.3">
+      <c r="A55" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F11" s="14" t="s">
+    <row r="56" spans="1:6" ht="39" x14ac:dyDescent="0.3">
+      <c r="A56" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C12" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="C13" s="23"/>
-      <c r="D13" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="14" t="s">
+    <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A57" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="E57" s="25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>329</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>330</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="14" t="s">
+      <c r="F57" s="24"/>
+    </row>
+    <row r="58" spans="1:6" ht="39" x14ac:dyDescent="0.3">
+      <c r="A58" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="E58" s="25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="14" t="s">
+      <c r="F58" s="24"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E59" s="25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="18" t="s">
+      <c r="F59" s="24"/>
+    </row>
+    <row r="60" spans="1:6" ht="39" x14ac:dyDescent="0.3">
+      <c r="A60" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E60" s="25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>211</v>
-      </c>
-      <c r="B57"/>
-      <c r="C57" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>217</v>
-      </c>
-      <c r="B58"/>
-      <c r="C58" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>218</v>
-      </c>
-      <c r="B59"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>219</v>
-      </c>
-      <c r="B60"/>
-      <c r="C60" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F60"/>
+      <c r="F60" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2996,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3010,7 +3134,7 @@
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>92</v>
       </c>
@@ -3029,8 +3153,26 @@
       <c r="F2" s="13" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G2" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
@@ -3038,13 +3180,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
         <v>10</v>
@@ -3057,10 +3199,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F44"/>
+  <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3074,7 +3216,7 @@
     <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>92</v>
       </c>
@@ -3082,7 +3224,7 @@
         <v>95</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>13</v>
@@ -3090,8 +3232,32 @@
       <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -3099,7 +3265,7 @@
         <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>90</v>
@@ -3108,12 +3274,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>267</v>
+    <row r="5" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>223</v>
@@ -3122,498 +3288,498 @@
         <v>222</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="15"/>
+      <c r="C8" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="C8" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="F9" s="21" t="s">
+      <c r="F10" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="377" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:14" ht="377" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
         <v>152</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>224</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>341</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>347</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>349</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
+    <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21" t="s">
-        <v>341</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>348</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
+      <c r="C22" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
-        <v>248</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>226</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
+      <c r="F24" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
+      <c r="C26" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
+      <c r="F27" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
+    </row>
+    <row r="30" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
+      <c r="F30" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E29" s="1" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E30" s="1" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="15" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="16" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="15" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="16" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="16" t="s">
-        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -3624,10 +3790,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3638,7 +3804,7 @@
     <col min="5" max="5" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -3651,8 +3817,26 @@
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="G1" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -3664,7 +3848,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3676,7 +3860,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -3688,7 +3872,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -3698,7 +3882,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3710,7 +3894,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -3720,7 +3904,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
@@ -3729,7 +3913,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
       <c r="D9" s="7" t="s">
         <v>73</v>
@@ -3745,7 +3929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3857,16 +4041,16 @@
     </row>
     <row r="10" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated workflows in requirements sheet and accordingly corrected few class names and their attributes
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="496">
   <si>
     <t>Term</t>
   </si>
@@ -1418,9 +1418,6 @@
     <t>Result 3</t>
   </si>
   <si>
-    <t>Product domain-Web Controller</t>
-  </si>
-  <si>
     <t>Product aggregate creation and update in ProductView read repo with status as "PENDING.</t>
   </si>
   <si>
@@ -1430,17 +1427,7 @@
     <t>Administrator sets/modifies inputs required for Forecast results calculation for each subscriptionable product</t>
   </si>
   <si>
-    <t>Product domain - Web controller</t>
-  </si>
-  <si>
     <t>ProductConfigurationValidator is invoked which checks if the complete configuration  inputs for correct product configuration are entered,when the out put is "true" then fire event "ProductConfigurationCompletedEvent".</t>
-  </si>
-  <si>
-    <t>ProductConfigurationCompletedEvent triggers forecast calculation event in case new forecast is being set for the first time.The completion of Forecast metrics calculation completion will trigger "ForecastMetricscalculatedEvent".
-ProductConfigurationComletedEvent should also trigger interpolation of monthly inputs to daily attributes inside InstantaneousPerformanceTracker list.</t>
-  </si>
-  <si>
-    <t>Administrator sets Rule parameters to subscriptionable item.(product level/basket level etc)</t>
   </si>
   <si>
     <t>Subscriber fills registration form to register on subscription website.</t>
@@ -1587,14 +1574,7 @@
     <t>Many aggregates are keeping big collections of forecasts/actuals as axon does not provide any API for maintaining versions(future/past) is there any way around it?</t>
   </si>
   <si>
-    <t>1. Admin uploads the CSV for products to be registered as subscriptionable items</t>
-  </si>
-  <si>
     <t>Integration domain-ProductRegistrationEvent (Camel Bindy) mapped to Product domain event</t>
-  </si>
-  <si>
-    <t>A New "ProductUploadedEvent" gets fired from write side to update same info on read side.
-The same event also notifies admin that remaining configuration of these fresh uploaded products need to be manually done.</t>
   </si>
   <si>
     <t>A Notification mail/sms to be sent to admin asking him to complete configuration of uploaded products with list of products for which config is incomplete.</t>
@@ -1626,14 +1606,6 @@
   </si>
   <si>
     <t>A CommonOperatingExpense aggregate instance is newly created from AddCommonOperatingExpenseCommand and all parameters( exp header,amount per month,sensitiveTo) are set in it.</t>
-  </si>
-  <si>
-    <t>Product aggregate updated with forecast inputs as well as Product view updated(?) with forecast inputs and status as "PENDING"if this is not the last activity of product configuration.
-Every change to product configuration,system should check if any more configuration is pending. If this is the last configuration fulfillment for the product then status is changed to"COMPLETE".</t>
-  </si>
-  <si>
-    <t>Product aggregate updated with rule inputs as well as Product view updated(?) with rule inputs and status as "PENDING"if this is not the last activity of product configuration.
-Every change to product configuration,system should check if any more configuration is pending. If this is the last configuration fulfillment for the product then status is changed to"COMPLETE".</t>
   </si>
   <si>
     <t>Each Product aggregate will get updated with OperatingExpensesPerUnit(which is sum of common expenses er unit and delivery charges per unit).The OperatingExpenseUpdatedEvent will get triggered which will update ProductView on read side.
@@ -1688,12 +1660,53 @@
 4.It will consolidate the delivery charges are product level and update Product aggregate's OperatingExpensePerUnit value.
 5.Save in the SubscriptionSpecificOperatingExpenseView.</t>
   </si>
+  <si>
+    <t>Product domain-ProductController-regsiterProduct</t>
+  </si>
+  <si>
+    <t>A New "ProductUploadedEvent" gets fired from write side to update same info on read side.
+The event updates ProductView on read side with status as "PENDING"as remaning configuration of the registered product is yet to be made.
+The same event also notifies admin that remaining configuration of these fresh uploaded products need to be manually done.</t>
+  </si>
+  <si>
+    <t>1. Admin registers product manually from adminConsole Web UI</t>
+  </si>
+  <si>
+    <t>Product domain - ProductController-addProjectionParamters.It will find out product from ProductView,create AddForecastParametersCommand and send it.</t>
+  </si>
+  <si>
+    <t>Product aggregate receives the command and fires ForecastParametersAddedEvent.It will update the ForecastedPerformanceView  through ForecastedPerformanceViewRepository with given inputs.</t>
+  </si>
+  <si>
+    <t>Product domain - ProductController-setProductConfiguration.It will find out product from ProductView,receive config params such as demand curve period,percentage revenue change for which price should be recalculated, is cross price elasticity to be considered, demand wise profit sharing percentage. It will send SetProductConfigurationCommand.</t>
+  </si>
+  <si>
+    <t>Product aggregate receives command and in turn fires ProductConfigurationSetEvent which updates ProductConfigurationView.</t>
+  </si>
+  <si>
+    <t>Administrator sets Configuration parameters for product level item.</t>
+  </si>
+  <si>
+    <t>Administrator sets configuration rules for Basket</t>
+  </si>
+  <si>
+    <t>Subscriber domain-BasketRulesController-addBasketRules.Following configuration rules are set at asket level
+1. Maximum permissible Basket amount
+2. Maximum permissible discount(percentage)
+3. Minimum amount for which basket is eligible for free shipping.</t>
+  </si>
+  <si>
+    <t>AddBasketRulesCommand if fired which sets configuration paramters in BasketRule view</t>
+  </si>
+  <si>
+    <t>OperatingExpenseUpdatedEvent triggers CalculateMetricsCommand (in case new forecast is being set for the first time).The MetricsCalculationProcessor calculates the resultant metrics for next 12 months for each product using the available input paramters for each.The completion of Forecast metrics calculation will trigger "ForecastMetricscalculatedEvent".It will update ForecastPerformanceView.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1740,6 +1753,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1841,11 +1860,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1959,10 +1975,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1971,7 +2002,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2330,10 +2364,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.1796875" style="2"/>
-    <col min="3" max="3" width="17.54296875" style="2"/>
-    <col min="4" max="4" width="102.453125" style="2"/>
-    <col min="5" max="1025" width="9.1796875" style="2"/>
+    <col min="1" max="2" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="17.54296875" style="1"/>
+    <col min="4" max="4" width="102.453125" style="1"/>
+    <col min="5" max="1025" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.35">
@@ -2341,66 +2375,66 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2421,1087 +2455,1087 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="5"/>
-    <col min="2" max="2" width="14.54296875" style="5"/>
-    <col min="3" max="3" width="16.26953125" style="5"/>
-    <col min="4" max="4" width="75.26953125" style="5"/>
-    <col min="5" max="7" width="16.26953125" style="5"/>
-    <col min="8" max="8" width="19.453125" style="5"/>
-    <col min="9" max="12" width="16.26953125" style="5"/>
-    <col min="13" max="13" width="17.26953125" style="5"/>
-    <col min="14" max="1025" width="16.26953125" style="5"/>
+    <col min="1" max="1" width="9.7265625" style="4"/>
+    <col min="2" max="2" width="14.54296875" style="4"/>
+    <col min="3" max="3" width="16.26953125" style="4"/>
+    <col min="4" max="4" width="75.26953125" style="4"/>
+    <col min="5" max="7" width="16.26953125" style="4"/>
+    <col min="8" max="8" width="19.453125" style="4"/>
+    <col min="9" max="12" width="16.26953125" style="4"/>
+    <col min="13" max="13" width="17.26953125" style="4"/>
+    <col min="14" max="1025" width="16.26953125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11" t="s">
+      <c r="L3" s="10"/>
+      <c r="M3" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:13" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="C6" s="15" t="s">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="C6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="C7" s="14"/>
+      <c r="D7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:13" s="8" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" ht="78.5" x14ac:dyDescent="0.35">
-      <c r="C10" s="15" t="s">
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="C10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11" t="s">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11" t="s">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="8" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="C12" s="20" t="s">
+    <row r="12" spans="1:13" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="C12" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="8" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="C13" s="20"/>
-      <c r="D13" s="21" t="s">
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="C13" s="19"/>
+      <c r="D13" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-    </row>
-    <row r="14" spans="1:13" s="8" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="C14" s="20"/>
-      <c r="D14" s="21" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="19"/>
+      <c r="D14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-    </row>
-    <row r="15" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:13" s="8" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="C16" s="20"/>
-      <c r="D16" s="21" t="s">
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:13" s="7" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="C17" s="20"/>
-      <c r="D17" s="21" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" s="7" customFormat="1" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="C17" s="19"/>
+      <c r="D17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="C18" s="20"/>
-      <c r="D18" s="21" t="s">
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" s="7" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="C18" s="19"/>
+      <c r="D18" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C19" s="20"/>
-      <c r="D19" s="22" t="s">
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C19" s="19"/>
+      <c r="D19" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="20"/>
-      <c r="D20" s="22" t="s">
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="19"/>
+      <c r="D20" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C21" s="20"/>
-      <c r="D21" s="22" t="s">
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C21" s="19"/>
+      <c r="D21" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-    </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="C22" s="20"/>
-      <c r="D22" s="22" t="s">
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C22" s="19"/>
+      <c r="D22" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="C23" s="20"/>
-      <c r="D23" s="20" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" s="8" customFormat="1" ht="78" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+    <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" s="7" customFormat="1" ht="78" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:6" s="7" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10" t="s">
+      <c r="E26" s="8"/>
+      <c r="F26" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:6" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9" t="s">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10" t="s">
+      <c r="E27" s="8"/>
+      <c r="F27" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:6" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="18" t="s">
+      <c r="E28" s="14"/>
+      <c r="F28" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" ht="78.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="17" t="s">
+    <row r="29" spans="1:6" s="7" customFormat="1" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="23" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A30" s="23" t="s">
+    <row r="30" spans="1:6" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24" t="s">
+      <c r="C30" s="23"/>
+      <c r="D30" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25" t="s">
+      <c r="E30" s="23"/>
+      <c r="F30" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10" t="s">
+      <c r="E31" s="8"/>
+      <c r="F31" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="52" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10" t="s">
+      <c r="E32" s="8"/>
+      <c r="F32" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10" t="s">
+      <c r="E33" s="8"/>
+      <c r="F33" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="15" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="18" t="s">
+      <c r="E34" s="14"/>
+      <c r="F34" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10" t="s">
+      <c r="E35" s="8"/>
+      <c r="F35" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="15" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="18" t="s">
+      <c r="E36" s="14"/>
+      <c r="F36" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10" t="s">
+      <c r="E37" s="8"/>
+      <c r="F37" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="15" t="s">
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="18" t="s">
+      <c r="E38" s="14"/>
+      <c r="F38" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="10" t="s">
+      <c r="E39" s="8"/>
+      <c r="F39" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="15" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="18" t="s">
+      <c r="E40" s="14"/>
+      <c r="F40" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10" t="s">
+      <c r="E41" s="8"/>
+      <c r="F41" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10" t="s">
+      <c r="E42" s="8"/>
+      <c r="F42" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="91" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E43" s="9"/>
-      <c r="F43" s="10" t="s">
+      <c r="E43" s="8"/>
+      <c r="F43" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="10" t="s">
+      <c r="E44" s="10"/>
+      <c r="F44" s="9" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="5" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="10" t="s">
+      <c r="E45" s="7"/>
+      <c r="F45" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="5" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="10" t="s">
+      <c r="E46" s="7"/>
+      <c r="F46" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="5" t="s">
+      <c r="E47" s="8"/>
+      <c r="F47" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9" t="s">
+      <c r="B48" s="7"/>
+      <c r="C48" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="5" t="s">
+      <c r="E48" s="8"/>
+      <c r="F48" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="5" t="s">
+      <c r="E49" s="8"/>
+      <c r="F49" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E50" s="9"/>
-      <c r="F50" s="5" t="s">
+      <c r="E50" s="8"/>
+      <c r="F50" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9" t="s">
+      <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="5" t="s">
+      <c r="E51" s="8"/>
+      <c r="F51" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="9"/>
-      <c r="F52" s="5" t="s">
+      <c r="E52" s="8"/>
+      <c r="F52" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="52" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="5" t="s">
+      <c r="E53" s="8"/>
+      <c r="F53" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24" t="s">
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="23" t="s">
+      <c r="E54" s="23"/>
+      <c r="F54" s="22" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="9" t="s">
+      <c r="B55" s="7"/>
+      <c r="C55" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E55" s="9"/>
-      <c r="F55" s="5" t="s">
+      <c r="E55" s="8"/>
+      <c r="F55" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9" t="s">
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="5" t="s">
+      <c r="E56" s="8"/>
+      <c r="F56" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="5" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="5" t="s">
+      <c r="E57" s="7"/>
+      <c r="F57" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9" t="s">
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E58" s="9"/>
-      <c r="F58" s="5" t="s">
+      <c r="E58" s="8"/>
+      <c r="F58" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="5" t="s">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="5" t="s">
+      <c r="E59" s="7"/>
+      <c r="F59" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="5" t="s">
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="5" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="5" t="s">
+      <c r="E61" s="7"/>
+      <c r="F61" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="5" t="s">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="5" t="s">
+      <c r="E62" s="7"/>
+      <c r="F62" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9" t="s">
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E63" s="9"/>
-      <c r="F63" s="5" t="s">
+      <c r="E63" s="8"/>
+      <c r="F63" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="5" t="s">
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="5" t="s">
+      <c r="E64" s="7"/>
+      <c r="F64" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="65" x14ac:dyDescent="0.35">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="5" t="s">
+      <c r="B65" s="7"/>
+      <c r="C65" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E65" s="8"/>
-      <c r="F65" s="10" t="s">
+      <c r="E65" s="7"/>
+      <c r="F65" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="10" t="s">
+      <c r="E66" s="7"/>
+      <c r="F66" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11" t="s">
+      <c r="B67" s="10"/>
+      <c r="C67" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F67" s="11"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68" spans="1:6" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11" t="s">
+      <c r="B68" s="10"/>
+      <c r="C68" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="D68" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="11"/>
+      <c r="F68" s="10"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11" t="s">
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F69" s="11"/>
+      <c r="F69" s="10"/>
     </row>
     <row r="70" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11" t="s">
+      <c r="B70" s="10"/>
+      <c r="C70" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="D70" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="E70" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F70" s="11"/>
+      <c r="F70" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3525,13 +3559,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" style="8"/>
-    <col min="2" max="2" width="11.1796875" style="8"/>
-    <col min="3" max="3" width="36.1796875" style="8"/>
-    <col min="4" max="4" width="52.81640625" style="8"/>
-    <col min="5" max="5" width="27.1796875" style="8"/>
-    <col min="6" max="6" width="17" style="8"/>
-    <col min="7" max="1025" width="8.54296875" style="8"/>
+    <col min="1" max="1" width="8.54296875" style="7"/>
+    <col min="2" max="2" width="11.1796875" style="7"/>
+    <col min="3" max="3" width="36.1796875" style="7"/>
+    <col min="4" max="4" width="52.81640625" style="7"/>
+    <col min="5" max="5" width="27.1796875" style="7"/>
+    <col min="6" max="6" width="17" style="7"/>
+    <col min="7" max="1025" width="8.54296875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -3549,76 +3583,76 @@
       <c r="L1"/>
     </row>
     <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>193</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="C4" s="26"/>
-      <c r="D4" s="26" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25" t="s">
         <v>194</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="26"/>
-      <c r="D5" s="26" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25" t="s">
         <v>195</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C6"/>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>196</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C7"/>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>197</v>
       </c>
       <c r="E7"/>
@@ -3629,10 +3663,10 @@
       <c r="E8"/>
     </row>
     <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>199</v>
       </c>
       <c r="E9"/>
@@ -3643,10 +3677,10 @@
       <c r="E10"/>
     </row>
     <row r="11" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>201</v>
       </c>
       <c r="E11"/>
@@ -3657,10 +3691,10 @@
       <c r="E12"/>
     </row>
     <row r="13" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="26" t="s">
         <v>203</v>
       </c>
       <c r="E13"/>
@@ -3671,43 +3705,43 @@
       <c r="E14"/>
     </row>
     <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="17" spans="4:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="26" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="18" spans="4:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="26" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="19" spans="4:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="20" spans="4:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="21" spans="4:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3728,88 +3762,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="28"/>
-    <col min="2" max="2" width="16.453125" style="28"/>
-    <col min="3" max="3" width="17.08984375" style="28"/>
-    <col min="4" max="4" width="44.26953125" style="28"/>
-    <col min="5" max="5" width="73.1796875" style="28"/>
-    <col min="6" max="6" width="12.453125" style="28"/>
-    <col min="7" max="7" width="11.1796875" style="28"/>
-    <col min="8" max="8" width="8.7265625" style="28"/>
-    <col min="9" max="9" width="24.90625" style="28"/>
-    <col min="10" max="10" width="22.7265625" style="28"/>
-    <col min="11" max="11" width="28.453125" style="28"/>
-    <col min="12" max="12" width="18" style="28"/>
-    <col min="13" max="13" width="8.7265625" style="28"/>
-    <col min="14" max="14" width="26.453125" style="28"/>
-    <col min="15" max="1025" width="8.7265625" style="28"/>
+    <col min="1" max="1" width="11.453125" style="27"/>
+    <col min="2" max="2" width="16.453125" style="27"/>
+    <col min="3" max="3" width="17.08984375" style="27"/>
+    <col min="4" max="4" width="44.26953125" style="27"/>
+    <col min="5" max="5" width="73.1796875" style="27"/>
+    <col min="6" max="6" width="12.453125" style="27"/>
+    <col min="7" max="7" width="11.1796875" style="27"/>
+    <col min="8" max="8" width="8.7265625" style="27"/>
+    <col min="9" max="9" width="24.90625" style="27"/>
+    <col min="10" max="10" width="22.7265625" style="27"/>
+    <col min="11" max="11" width="28.453125" style="27"/>
+    <col min="12" max="12" width="18" style="27"/>
+    <col min="13" max="13" width="8.7265625" style="27"/>
+    <col min="14" max="14" width="26.453125" style="27"/>
+    <col min="15" max="1025" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3"/>
       <c r="I3"/>
       <c r="J3"/>
@@ -3818,131 +3852,131 @@
       <c r="N3"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="26" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="26" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="26" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>51</v>
       </c>
       <c r="I7"/>
@@ -3952,508 +3986,508 @@
       <c r="N7"/>
     </row>
     <row r="8" spans="1:14" ht="290" x14ac:dyDescent="0.35">
-      <c r="A8" s="32"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="28" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="L8" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="N8" s="28" t="s">
+      <c r="N8" s="27" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="32" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="377" x14ac:dyDescent="0.35">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="28" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="28" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="27" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>291</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="27" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>294</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="27" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="27" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="27" t="s">
         <v>320</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="27" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="27" t="s">
         <v>323</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="27" t="s">
         <v>324</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="27" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="27" t="s">
         <v>326</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="27" t="s">
         <v>327</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="27" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="27" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="27" t="s">
         <v>333</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="27" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="21" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="21" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="21" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="21" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="31" t="s">
         <v>343</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="21" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="21" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="31" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="31" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="31" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="31" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="31" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="31" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="31" t="s">
         <v>354</v>
       </c>
     </row>
@@ -4488,28 +4522,28 @@
       <c r="B1" t="s">
         <v>355</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4517,23 +4551,23 @@
       <c r="A2" t="s">
         <v>356</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="E2" s="35"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4541,61 +4575,61 @@
       <c r="A4" t="s">
         <v>362</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>366</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>367</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="E6" s="35"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>369</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:12" ht="87" x14ac:dyDescent="0.35">
-      <c r="C9" s="35"/>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4613,12 +4647,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="2"/>
-    <col min="2" max="2" width="15.7265625" style="2"/>
-    <col min="3" max="3" width="47.81640625" style="2"/>
-    <col min="4" max="4" width="37.7265625" style="2"/>
-    <col min="5" max="5" width="79.08984375" style="2"/>
-    <col min="6" max="1025" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="15.7265625" style="1"/>
+    <col min="3" max="3" width="47.81640625" style="1"/>
+    <col min="4" max="4" width="37.7265625" style="1"/>
+    <col min="5" max="5" width="79.08984375" style="1"/>
+    <col min="6" max="1025" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -4630,19 +4664,19 @@
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -4654,104 +4688,104 @@
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B4"/>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>374</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B5"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>377</v>
       </c>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>378</v>
       </c>
       <c r="B6"/>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>380</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>381</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>384</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B8"/>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>392</v>
       </c>
     </row>
@@ -4781,82 +4815,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="33" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="174" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="37" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>396</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="37" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>401</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="37" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4874,10 +4908,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4887,369 +4921,384 @@
     <col min="3" max="3" width="53.08984375" customWidth="1"/>
     <col min="4" max="4" width="45.90625" customWidth="1"/>
     <col min="5" max="5" width="52.08984375" customWidth="1"/>
-    <col min="6" max="6" width="35.1796875" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="6" max="6" width="53.36328125" customWidth="1"/>
+    <col min="7" max="7" width="87.08984375" customWidth="1"/>
     <col min="8" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>406</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>408</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="43" t="s">
+        <v>470</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>486</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>484</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>411</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>485</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="A3" s="39">
+        <v>1</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>461</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>411</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="G3" s="44"/>
+    </row>
+    <row r="4" spans="1:7" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="49" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>487</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>488</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>414</v>
+      </c>
+      <c r="G4" s="46"/>
+    </row>
+    <row r="5" spans="1:7" ht="91" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="49" t="s">
+        <v>491</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>489</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>490</v>
+      </c>
+      <c r="F5" s="50"/>
+      <c r="G5" s="46"/>
+    </row>
+    <row r="6" spans="1:7" ht="91" x14ac:dyDescent="0.35">
+      <c r="A6" s="41"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="49" t="s">
+        <v>492</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>493</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>494</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="42"/>
+    </row>
+    <row r="7" spans="1:7" ht="104" x14ac:dyDescent="0.35">
+      <c r="A7" s="39"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="39" t="s">
+        <v>466</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>463</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>471</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A8" s="39"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="39" t="s">
+        <v>468</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>463</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>467</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="1:7" ht="169" x14ac:dyDescent="0.35">
+      <c r="A9" s="39"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="39" t="s">
+        <v>481</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>480</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>472</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>495</v>
+      </c>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A10" s="39">
+        <v>2</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>415</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>417</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>418</v>
+      </c>
+      <c r="G10" s="39"/>
+    </row>
+    <row r="11" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A11" s="39"/>
+      <c r="B11" s="45" t="s">
+        <v>419</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>420</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>421</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>473</v>
+      </c>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="A12" s="39"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="39" t="s">
+        <v>422</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>423</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>424</v>
+      </c>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A13" s="39"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="39" t="s">
+        <v>425</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>426</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" ht="104" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="39" t="s">
+        <v>428</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>474</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" spans="1:7" ht="78" x14ac:dyDescent="0.35">
+      <c r="A15" s="39"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="39" t="s">
+        <v>430</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>431</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>475</v>
+      </c>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+    </row>
+    <row r="16" spans="1:7" ht="65" x14ac:dyDescent="0.35">
+      <c r="A16" s="39"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="39" t="s">
+        <v>432</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>434</v>
+      </c>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+    </row>
+    <row r="17" spans="1:7" ht="52" x14ac:dyDescent="0.35">
+      <c r="A17" s="39"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>435</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>436</v>
+      </c>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+    </row>
+    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A18" s="39"/>
+      <c r="B18" s="39" t="s">
+        <v>437</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>438</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>439</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>440</v>
+      </c>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+    </row>
+    <row r="19" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39" t="s">
+        <v>441</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>442</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>443</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>444</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" ht="78" x14ac:dyDescent="0.35">
+      <c r="A20" s="39"/>
+      <c r="B20" s="43" t="s">
         <v>476</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>465</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>411</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>412</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A3" s="40">
-        <v>1</v>
-      </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="40" t="s">
-        <v>413</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>466</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>412</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="42"/>
-    </row>
-    <row r="4" spans="1:7" ht="91" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="40" t="s">
-        <v>414</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="E4" s="40" t="s">
+      <c r="C20" s="39" t="s">
+        <v>477</v>
+      </c>
+      <c r="D20" s="39" t="s">
         <v>478</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="91" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="40" t="s">
-        <v>418</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="E5" s="40" t="s">
+      <c r="E20" s="39" t="s">
         <v>479</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="104" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="40" t="s">
-        <v>472</v>
-      </c>
-      <c r="D6" s="40" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+    </row>
+    <row r="21" spans="1:7" ht="234" x14ac:dyDescent="0.35">
+      <c r="A21" s="39"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>483</v>
+      </c>
+      <c r="E21" s="39" t="s">
         <v>469</v>
       </c>
-      <c r="E6" s="40" t="s">
-        <v>477</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>470</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="52" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="40" t="s">
-        <v>474</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>469</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>473</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-    </row>
-    <row r="8" spans="1:7" ht="195" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="40" t="s">
-        <v>489</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>488</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>480</v>
-      </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-    </row>
-    <row r="9" spans="1:7" ht="52" x14ac:dyDescent="0.35">
-      <c r="A9" s="40">
-        <v>2</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>419</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>420</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>421</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>422</v>
-      </c>
-      <c r="G9" s="40"/>
-    </row>
-    <row r="10" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>424</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>425</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>481</v>
-      </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-    </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="40" t="s">
-        <v>426</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>427</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>428</v>
-      </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-    </row>
-    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="40" t="s">
-        <v>429</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>430</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>431</v>
-      </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-    </row>
-    <row r="13" spans="1:7" ht="104" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="40" t="s">
-        <v>432</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>433</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>482</v>
-      </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-    </row>
-    <row r="14" spans="1:7" ht="78" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="40" t="s">
-        <v>434</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>435</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>483</v>
-      </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-    </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="40" t="s">
-        <v>436</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>437</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>438</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-    </row>
-    <row r="16" spans="1:7" ht="52" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>439</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>440</v>
-      </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-    </row>
-    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40" t="s">
-        <v>441</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>442</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>443</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>444</v>
-      </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-    </row>
-    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40" t="s">
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+    </row>
+    <row r="22" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A22" s="39"/>
+      <c r="B22" s="39" t="s">
         <v>445</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>446</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>447</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>448</v>
-      </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-    </row>
-    <row r="19" spans="1:7" ht="78" x14ac:dyDescent="0.35">
-      <c r="A19" s="40"/>
-      <c r="B19" s="41" t="s">
-        <v>484</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>486</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>487</v>
-      </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-    </row>
-    <row r="20" spans="1:7" ht="247" x14ac:dyDescent="0.35">
-      <c r="A20" s="40"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="40" t="s">
-        <v>490</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>491</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>475</v>
-      </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-    </row>
-    <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40" t="s">
-        <v>449</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="B11:B17"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B2:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -5279,7 +5328,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -5287,7 +5336,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -5295,23 +5344,23 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>453</v>
+      <c r="B5" s="7" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>454</v>
+      <c r="B6" s="7" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -5319,79 +5368,79 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>456</v>
+      <c r="B8" s="7" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>457</v>
+      <c r="B9" s="7" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>458</v>
+      <c r="B10" s="7" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>459</v>
+      <c r="B11" s="7" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>460</v>
+      <c r="B12" s="7" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>461</v>
+      <c r="B13" s="7" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>462</v>
+      <c r="B14" s="7" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>463</v>
+      <c r="B15" s="7" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>464</v>
+      <c r="B16" s="7" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added partial AI in workflow. Added BAM requirements for product category (pending for customer and business).
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.003.xlsx
@@ -17,14 +17,14 @@
     <sheet name="PaymentMode" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="workflows" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Sheet2" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="BAN" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="BAM" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="513">
   <si>
     <t>Term</t>
   </si>
@@ -1415,6 +1415,9 @@
     <t>Result 3</t>
   </si>
   <si>
+    <t>Action Item</t>
+  </si>
+  <si>
     <t>Item Registration &amp; Product configuration &amp; Forecasting</t>
   </si>
   <si>
@@ -1430,6 +1433,9 @@
     <t>A New "ProductRegisteredEvent" gets fired from write side to update same info on read side.
 The event updates ProductView on read side with status as "REGISTERED" as remaning configuration of the registered product is yet to be made.
 The same event also notifies admin that remaining configuration of these fresh uploaded products need to be manually done.</t>
+  </si>
+  <si>
+    <t>Anayonkar</t>
   </si>
   <si>
     <t>2. Platform periodically receives list of new product details  for registering them as subscriptioable Items from shopping site.</t>
@@ -1493,7 +1499,7 @@
 In the listener, DeliveryChargesRuleViewRepository is instantiated from controller,For each delivery charge rule a DeliveryChargesRuleView is created and stored in the repository.</t>
   </si>
   <si>
-    <t>A ExpenseDistributionBatch is instantiated initially and invokes CommonExpenseDistributionProcessor and SubscriptionSpecificExpenseDistributionProcessor for distribution of respective exepnses across all the subscribed as well as forecasted subscribed units for registered products. </t>
+    <t>A ExpenseDistributionBatch is instantiated initially and invokes CommonExpenseDistributionProcessor and SubscriptionSpecificExpenseDistributionProcessor for distribution of respective exepnses across all the subscribed as well as forecasted subscribed units for registered products.</t>
   </si>
   <si>
     <r>
@@ -1518,8 +1524,10 @@
   </si>
   <si>
     <t>Each Product aggregate will get updated with OperatingExpensesPerUnit(which is sum of common expenses er unit and delivery charges per unit).The OperatingExpenseUpdatedEvent will get triggered which will update ProductView on read side.
-Status of product in product view will be marked as "COMPLETE"
-</t>
+Status of product in product view will be marked as "COMPLETE"</t>
+  </si>
+  <si>
+    <t>Rahul</t>
   </si>
   <si>
     <t>A ProductPricingBatch is instantiated which will use the configuration rules and calculated expenses to derive price of each product</t>
@@ -1532,6 +1540,9 @@
   </si>
   <si>
     <t>ProductPriceCalculatedEvent triggers CalculateMetricsCommand (in case new forecast is being set for the first time).The MetricsCalculationProcessor calculates the resultant metrics for next 12 months for each product using the available input paramters for each.The completion of Forecast metrics calculation will trigger "ForecastMetricscalculatedEvent".It will update ForecastPerformanceView.</t>
+  </si>
+  <si>
+    <t>Mandar</t>
   </si>
   <si>
     <t>Subscriber fills registration form to register on subscription website.</t>
@@ -1654,7 +1665,7 @@
 If the expense tye is SubscriptionSpecificOperatingExpense then it is updated in SubscriptionSpecificOperatingExpenseView.</t>
   </si>
   <si>
-    <t>A ExpenseDistributionBatch is instantiated On receipt of OperatingExpenseReceivedEvent and invokes CommonExpenseDistributionProcessor and SubscriptionSpecificExpenseDistributionProcessor for distribution of respective exepnses across all the subscribed as well as forecasted subscribed units for registered products. </t>
+    <t>A ExpenseDistributionBatch is instantiated On receipt of OperatingExpenseReceivedEvent and invokes CommonExpenseDistributionProcessor and SubscriptionSpecificExpenseDistributionProcessor for distribution of respective exepnses across all the subscribed as well as forecasted subscribed units for registered products.</t>
   </si>
   <si>
     <t>CommonExpenseDistributionProcessor will
@@ -1717,6 +1728,42 @@
   </si>
   <si>
     <t>Many aggregates are keeping big collections of forecasts/actuals as axon does not provide any API for maintaining versions(future/past) is there any way around it?</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Category (Business/ Customer/ Product)</t>
+  </si>
+  <si>
+    <t>Comments/Details</t>
+  </si>
+  <si>
+    <t>Impacted by user story</t>
+  </si>
+  <si>
+    <t>High performing product</t>
+  </si>
+  <si>
+    <t>Admin is able to see specific product(s) which are performing better than forecast</t>
+  </si>
+  <si>
+    <t>Low performing product</t>
+  </si>
+  <si>
+    <t>Admin is able to see specific product(s) which are performing worse than forecast</t>
+  </si>
+  <si>
+    <t>Product pending configuration</t>
+  </si>
+  <si>
+    <t>Admin is able to see specific product(s) which are pending to complete the configuration (e.g. forecast not added etc.)</t>
+  </si>
+  <si>
+    <t>Product pending reconfiguration</t>
+  </si>
+  <si>
+    <t>Admin is able to see specific product(s) which are pending to complete the reconfiguration (e.g. forecast and expense distribution needs to be changed/reconfigured etc.)</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1926,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2036,8 +2083,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2050,6 +2105,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2227,17 +2286,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.5384615384615"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="31.2267206477733"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="24.1214574898785"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="9.1417004048583"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="45" t="s">
+        <v>501</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>503</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2313,7 +2435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -2327,6 +2449,1017 @@
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
+      <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
+      <c r="IX2" s="0"/>
+      <c r="IY2" s="0"/>
+      <c r="IZ2" s="0"/>
+      <c r="JA2" s="0"/>
+      <c r="JB2" s="0"/>
+      <c r="JC2" s="0"/>
+      <c r="JD2" s="0"/>
+      <c r="JE2" s="0"/>
+      <c r="JF2" s="0"/>
+      <c r="JG2" s="0"/>
+      <c r="JH2" s="0"/>
+      <c r="JI2" s="0"/>
+      <c r="JJ2" s="0"/>
+      <c r="JK2" s="0"/>
+      <c r="JL2" s="0"/>
+      <c r="JM2" s="0"/>
+      <c r="JN2" s="0"/>
+      <c r="JO2" s="0"/>
+      <c r="JP2" s="0"/>
+      <c r="JQ2" s="0"/>
+      <c r="JR2" s="0"/>
+      <c r="JS2" s="0"/>
+      <c r="JT2" s="0"/>
+      <c r="JU2" s="0"/>
+      <c r="JV2" s="0"/>
+      <c r="JW2" s="0"/>
+      <c r="JX2" s="0"/>
+      <c r="JY2" s="0"/>
+      <c r="JZ2" s="0"/>
+      <c r="KA2" s="0"/>
+      <c r="KB2" s="0"/>
+      <c r="KC2" s="0"/>
+      <c r="KD2" s="0"/>
+      <c r="KE2" s="0"/>
+      <c r="KF2" s="0"/>
+      <c r="KG2" s="0"/>
+      <c r="KH2" s="0"/>
+      <c r="KI2" s="0"/>
+      <c r="KJ2" s="0"/>
+      <c r="KK2" s="0"/>
+      <c r="KL2" s="0"/>
+      <c r="KM2" s="0"/>
+      <c r="KN2" s="0"/>
+      <c r="KO2" s="0"/>
+      <c r="KP2" s="0"/>
+      <c r="KQ2" s="0"/>
+      <c r="KR2" s="0"/>
+      <c r="KS2" s="0"/>
+      <c r="KT2" s="0"/>
+      <c r="KU2" s="0"/>
+      <c r="KV2" s="0"/>
+      <c r="KW2" s="0"/>
+      <c r="KX2" s="0"/>
+      <c r="KY2" s="0"/>
+      <c r="KZ2" s="0"/>
+      <c r="LA2" s="0"/>
+      <c r="LB2" s="0"/>
+      <c r="LC2" s="0"/>
+      <c r="LD2" s="0"/>
+      <c r="LE2" s="0"/>
+      <c r="LF2" s="0"/>
+      <c r="LG2" s="0"/>
+      <c r="LH2" s="0"/>
+      <c r="LI2" s="0"/>
+      <c r="LJ2" s="0"/>
+      <c r="LK2" s="0"/>
+      <c r="LL2" s="0"/>
+      <c r="LM2" s="0"/>
+      <c r="LN2" s="0"/>
+      <c r="LO2" s="0"/>
+      <c r="LP2" s="0"/>
+      <c r="LQ2" s="0"/>
+      <c r="LR2" s="0"/>
+      <c r="LS2" s="0"/>
+      <c r="LT2" s="0"/>
+      <c r="LU2" s="0"/>
+      <c r="LV2" s="0"/>
+      <c r="LW2" s="0"/>
+      <c r="LX2" s="0"/>
+      <c r="LY2" s="0"/>
+      <c r="LZ2" s="0"/>
+      <c r="MA2" s="0"/>
+      <c r="MB2" s="0"/>
+      <c r="MC2" s="0"/>
+      <c r="MD2" s="0"/>
+      <c r="ME2" s="0"/>
+      <c r="MF2" s="0"/>
+      <c r="MG2" s="0"/>
+      <c r="MH2" s="0"/>
+      <c r="MI2" s="0"/>
+      <c r="MJ2" s="0"/>
+      <c r="MK2" s="0"/>
+      <c r="ML2" s="0"/>
+      <c r="MM2" s="0"/>
+      <c r="MN2" s="0"/>
+      <c r="MO2" s="0"/>
+      <c r="MP2" s="0"/>
+      <c r="MQ2" s="0"/>
+      <c r="MR2" s="0"/>
+      <c r="MS2" s="0"/>
+      <c r="MT2" s="0"/>
+      <c r="MU2" s="0"/>
+      <c r="MV2" s="0"/>
+      <c r="MW2" s="0"/>
+      <c r="MX2" s="0"/>
+      <c r="MY2" s="0"/>
+      <c r="MZ2" s="0"/>
+      <c r="NA2" s="0"/>
+      <c r="NB2" s="0"/>
+      <c r="NC2" s="0"/>
+      <c r="ND2" s="0"/>
+      <c r="NE2" s="0"/>
+      <c r="NF2" s="0"/>
+      <c r="NG2" s="0"/>
+      <c r="NH2" s="0"/>
+      <c r="NI2" s="0"/>
+      <c r="NJ2" s="0"/>
+      <c r="NK2" s="0"/>
+      <c r="NL2" s="0"/>
+      <c r="NM2" s="0"/>
+      <c r="NN2" s="0"/>
+      <c r="NO2" s="0"/>
+      <c r="NP2" s="0"/>
+      <c r="NQ2" s="0"/>
+      <c r="NR2" s="0"/>
+      <c r="NS2" s="0"/>
+      <c r="NT2" s="0"/>
+      <c r="NU2" s="0"/>
+      <c r="NV2" s="0"/>
+      <c r="NW2" s="0"/>
+      <c r="NX2" s="0"/>
+      <c r="NY2" s="0"/>
+      <c r="NZ2" s="0"/>
+      <c r="OA2" s="0"/>
+      <c r="OB2" s="0"/>
+      <c r="OC2" s="0"/>
+      <c r="OD2" s="0"/>
+      <c r="OE2" s="0"/>
+      <c r="OF2" s="0"/>
+      <c r="OG2" s="0"/>
+      <c r="OH2" s="0"/>
+      <c r="OI2" s="0"/>
+      <c r="OJ2" s="0"/>
+      <c r="OK2" s="0"/>
+      <c r="OL2" s="0"/>
+      <c r="OM2" s="0"/>
+      <c r="ON2" s="0"/>
+      <c r="OO2" s="0"/>
+      <c r="OP2" s="0"/>
+      <c r="OQ2" s="0"/>
+      <c r="OR2" s="0"/>
+      <c r="OS2" s="0"/>
+      <c r="OT2" s="0"/>
+      <c r="OU2" s="0"/>
+      <c r="OV2" s="0"/>
+      <c r="OW2" s="0"/>
+      <c r="OX2" s="0"/>
+      <c r="OY2" s="0"/>
+      <c r="OZ2" s="0"/>
+      <c r="PA2" s="0"/>
+      <c r="PB2" s="0"/>
+      <c r="PC2" s="0"/>
+      <c r="PD2" s="0"/>
+      <c r="PE2" s="0"/>
+      <c r="PF2" s="0"/>
+      <c r="PG2" s="0"/>
+      <c r="PH2" s="0"/>
+      <c r="PI2" s="0"/>
+      <c r="PJ2" s="0"/>
+      <c r="PK2" s="0"/>
+      <c r="PL2" s="0"/>
+      <c r="PM2" s="0"/>
+      <c r="PN2" s="0"/>
+      <c r="PO2" s="0"/>
+      <c r="PP2" s="0"/>
+      <c r="PQ2" s="0"/>
+      <c r="PR2" s="0"/>
+      <c r="PS2" s="0"/>
+      <c r="PT2" s="0"/>
+      <c r="PU2" s="0"/>
+      <c r="PV2" s="0"/>
+      <c r="PW2" s="0"/>
+      <c r="PX2" s="0"/>
+      <c r="PY2" s="0"/>
+      <c r="PZ2" s="0"/>
+      <c r="QA2" s="0"/>
+      <c r="QB2" s="0"/>
+      <c r="QC2" s="0"/>
+      <c r="QD2" s="0"/>
+      <c r="QE2" s="0"/>
+      <c r="QF2" s="0"/>
+      <c r="QG2" s="0"/>
+      <c r="QH2" s="0"/>
+      <c r="QI2" s="0"/>
+      <c r="QJ2" s="0"/>
+      <c r="QK2" s="0"/>
+      <c r="QL2" s="0"/>
+      <c r="QM2" s="0"/>
+      <c r="QN2" s="0"/>
+      <c r="QO2" s="0"/>
+      <c r="QP2" s="0"/>
+      <c r="QQ2" s="0"/>
+      <c r="QR2" s="0"/>
+      <c r="QS2" s="0"/>
+      <c r="QT2" s="0"/>
+      <c r="QU2" s="0"/>
+      <c r="QV2" s="0"/>
+      <c r="QW2" s="0"/>
+      <c r="QX2" s="0"/>
+      <c r="QY2" s="0"/>
+      <c r="QZ2" s="0"/>
+      <c r="RA2" s="0"/>
+      <c r="RB2" s="0"/>
+      <c r="RC2" s="0"/>
+      <c r="RD2" s="0"/>
+      <c r="RE2" s="0"/>
+      <c r="RF2" s="0"/>
+      <c r="RG2" s="0"/>
+      <c r="RH2" s="0"/>
+      <c r="RI2" s="0"/>
+      <c r="RJ2" s="0"/>
+      <c r="RK2" s="0"/>
+      <c r="RL2" s="0"/>
+      <c r="RM2" s="0"/>
+      <c r="RN2" s="0"/>
+      <c r="RO2" s="0"/>
+      <c r="RP2" s="0"/>
+      <c r="RQ2" s="0"/>
+      <c r="RR2" s="0"/>
+      <c r="RS2" s="0"/>
+      <c r="RT2" s="0"/>
+      <c r="RU2" s="0"/>
+      <c r="RV2" s="0"/>
+      <c r="RW2" s="0"/>
+      <c r="RX2" s="0"/>
+      <c r="RY2" s="0"/>
+      <c r="RZ2" s="0"/>
+      <c r="SA2" s="0"/>
+      <c r="SB2" s="0"/>
+      <c r="SC2" s="0"/>
+      <c r="SD2" s="0"/>
+      <c r="SE2" s="0"/>
+      <c r="SF2" s="0"/>
+      <c r="SG2" s="0"/>
+      <c r="SH2" s="0"/>
+      <c r="SI2" s="0"/>
+      <c r="SJ2" s="0"/>
+      <c r="SK2" s="0"/>
+      <c r="SL2" s="0"/>
+      <c r="SM2" s="0"/>
+      <c r="SN2" s="0"/>
+      <c r="SO2" s="0"/>
+      <c r="SP2" s="0"/>
+      <c r="SQ2" s="0"/>
+      <c r="SR2" s="0"/>
+      <c r="SS2" s="0"/>
+      <c r="ST2" s="0"/>
+      <c r="SU2" s="0"/>
+      <c r="SV2" s="0"/>
+      <c r="SW2" s="0"/>
+      <c r="SX2" s="0"/>
+      <c r="SY2" s="0"/>
+      <c r="SZ2" s="0"/>
+      <c r="TA2" s="0"/>
+      <c r="TB2" s="0"/>
+      <c r="TC2" s="0"/>
+      <c r="TD2" s="0"/>
+      <c r="TE2" s="0"/>
+      <c r="TF2" s="0"/>
+      <c r="TG2" s="0"/>
+      <c r="TH2" s="0"/>
+      <c r="TI2" s="0"/>
+      <c r="TJ2" s="0"/>
+      <c r="TK2" s="0"/>
+      <c r="TL2" s="0"/>
+      <c r="TM2" s="0"/>
+      <c r="TN2" s="0"/>
+      <c r="TO2" s="0"/>
+      <c r="TP2" s="0"/>
+      <c r="TQ2" s="0"/>
+      <c r="TR2" s="0"/>
+      <c r="TS2" s="0"/>
+      <c r="TT2" s="0"/>
+      <c r="TU2" s="0"/>
+      <c r="TV2" s="0"/>
+      <c r="TW2" s="0"/>
+      <c r="TX2" s="0"/>
+      <c r="TY2" s="0"/>
+      <c r="TZ2" s="0"/>
+      <c r="UA2" s="0"/>
+      <c r="UB2" s="0"/>
+      <c r="UC2" s="0"/>
+      <c r="UD2" s="0"/>
+      <c r="UE2" s="0"/>
+      <c r="UF2" s="0"/>
+      <c r="UG2" s="0"/>
+      <c r="UH2" s="0"/>
+      <c r="UI2" s="0"/>
+      <c r="UJ2" s="0"/>
+      <c r="UK2" s="0"/>
+      <c r="UL2" s="0"/>
+      <c r="UM2" s="0"/>
+      <c r="UN2" s="0"/>
+      <c r="UO2" s="0"/>
+      <c r="UP2" s="0"/>
+      <c r="UQ2" s="0"/>
+      <c r="UR2" s="0"/>
+      <c r="US2" s="0"/>
+      <c r="UT2" s="0"/>
+      <c r="UU2" s="0"/>
+      <c r="UV2" s="0"/>
+      <c r="UW2" s="0"/>
+      <c r="UX2" s="0"/>
+      <c r="UY2" s="0"/>
+      <c r="UZ2" s="0"/>
+      <c r="VA2" s="0"/>
+      <c r="VB2" s="0"/>
+      <c r="VC2" s="0"/>
+      <c r="VD2" s="0"/>
+      <c r="VE2" s="0"/>
+      <c r="VF2" s="0"/>
+      <c r="VG2" s="0"/>
+      <c r="VH2" s="0"/>
+      <c r="VI2" s="0"/>
+      <c r="VJ2" s="0"/>
+      <c r="VK2" s="0"/>
+      <c r="VL2" s="0"/>
+      <c r="VM2" s="0"/>
+      <c r="VN2" s="0"/>
+      <c r="VO2" s="0"/>
+      <c r="VP2" s="0"/>
+      <c r="VQ2" s="0"/>
+      <c r="VR2" s="0"/>
+      <c r="VS2" s="0"/>
+      <c r="VT2" s="0"/>
+      <c r="VU2" s="0"/>
+      <c r="VV2" s="0"/>
+      <c r="VW2" s="0"/>
+      <c r="VX2" s="0"/>
+      <c r="VY2" s="0"/>
+      <c r="VZ2" s="0"/>
+      <c r="WA2" s="0"/>
+      <c r="WB2" s="0"/>
+      <c r="WC2" s="0"/>
+      <c r="WD2" s="0"/>
+      <c r="WE2" s="0"/>
+      <c r="WF2" s="0"/>
+      <c r="WG2" s="0"/>
+      <c r="WH2" s="0"/>
+      <c r="WI2" s="0"/>
+      <c r="WJ2" s="0"/>
+      <c r="WK2" s="0"/>
+      <c r="WL2" s="0"/>
+      <c r="WM2" s="0"/>
+      <c r="WN2" s="0"/>
+      <c r="WO2" s="0"/>
+      <c r="WP2" s="0"/>
+      <c r="WQ2" s="0"/>
+      <c r="WR2" s="0"/>
+      <c r="WS2" s="0"/>
+      <c r="WT2" s="0"/>
+      <c r="WU2" s="0"/>
+      <c r="WV2" s="0"/>
+      <c r="WW2" s="0"/>
+      <c r="WX2" s="0"/>
+      <c r="WY2" s="0"/>
+      <c r="WZ2" s="0"/>
+      <c r="XA2" s="0"/>
+      <c r="XB2" s="0"/>
+      <c r="XC2" s="0"/>
+      <c r="XD2" s="0"/>
+      <c r="XE2" s="0"/>
+      <c r="XF2" s="0"/>
+      <c r="XG2" s="0"/>
+      <c r="XH2" s="0"/>
+      <c r="XI2" s="0"/>
+      <c r="XJ2" s="0"/>
+      <c r="XK2" s="0"/>
+      <c r="XL2" s="0"/>
+      <c r="XM2" s="0"/>
+      <c r="XN2" s="0"/>
+      <c r="XO2" s="0"/>
+      <c r="XP2" s="0"/>
+      <c r="XQ2" s="0"/>
+      <c r="XR2" s="0"/>
+      <c r="XS2" s="0"/>
+      <c r="XT2" s="0"/>
+      <c r="XU2" s="0"/>
+      <c r="XV2" s="0"/>
+      <c r="XW2" s="0"/>
+      <c r="XX2" s="0"/>
+      <c r="XY2" s="0"/>
+      <c r="XZ2" s="0"/>
+      <c r="YA2" s="0"/>
+      <c r="YB2" s="0"/>
+      <c r="YC2" s="0"/>
+      <c r="YD2" s="0"/>
+      <c r="YE2" s="0"/>
+      <c r="YF2" s="0"/>
+      <c r="YG2" s="0"/>
+      <c r="YH2" s="0"/>
+      <c r="YI2" s="0"/>
+      <c r="YJ2" s="0"/>
+      <c r="YK2" s="0"/>
+      <c r="YL2" s="0"/>
+      <c r="YM2" s="0"/>
+      <c r="YN2" s="0"/>
+      <c r="YO2" s="0"/>
+      <c r="YP2" s="0"/>
+      <c r="YQ2" s="0"/>
+      <c r="YR2" s="0"/>
+      <c r="YS2" s="0"/>
+      <c r="YT2" s="0"/>
+      <c r="YU2" s="0"/>
+      <c r="YV2" s="0"/>
+      <c r="YW2" s="0"/>
+      <c r="YX2" s="0"/>
+      <c r="YY2" s="0"/>
+      <c r="YZ2" s="0"/>
+      <c r="ZA2" s="0"/>
+      <c r="ZB2" s="0"/>
+      <c r="ZC2" s="0"/>
+      <c r="ZD2" s="0"/>
+      <c r="ZE2" s="0"/>
+      <c r="ZF2" s="0"/>
+      <c r="ZG2" s="0"/>
+      <c r="ZH2" s="0"/>
+      <c r="ZI2" s="0"/>
+      <c r="ZJ2" s="0"/>
+      <c r="ZK2" s="0"/>
+      <c r="ZL2" s="0"/>
+      <c r="ZM2" s="0"/>
+      <c r="ZN2" s="0"/>
+      <c r="ZO2" s="0"/>
+      <c r="ZP2" s="0"/>
+      <c r="ZQ2" s="0"/>
+      <c r="ZR2" s="0"/>
+      <c r="ZS2" s="0"/>
+      <c r="ZT2" s="0"/>
+      <c r="ZU2" s="0"/>
+      <c r="ZV2" s="0"/>
+      <c r="ZW2" s="0"/>
+      <c r="ZX2" s="0"/>
+      <c r="ZY2" s="0"/>
+      <c r="ZZ2" s="0"/>
+      <c r="AAA2" s="0"/>
+      <c r="AAB2" s="0"/>
+      <c r="AAC2" s="0"/>
+      <c r="AAD2" s="0"/>
+      <c r="AAE2" s="0"/>
+      <c r="AAF2" s="0"/>
+      <c r="AAG2" s="0"/>
+      <c r="AAH2" s="0"/>
+      <c r="AAI2" s="0"/>
+      <c r="AAJ2" s="0"/>
+      <c r="AAK2" s="0"/>
+      <c r="AAL2" s="0"/>
+      <c r="AAM2" s="0"/>
+      <c r="AAN2" s="0"/>
+      <c r="AAO2" s="0"/>
+      <c r="AAP2" s="0"/>
+      <c r="AAQ2" s="0"/>
+      <c r="AAR2" s="0"/>
+      <c r="AAS2" s="0"/>
+      <c r="AAT2" s="0"/>
+      <c r="AAU2" s="0"/>
+      <c r="AAV2" s="0"/>
+      <c r="AAW2" s="0"/>
+      <c r="AAX2" s="0"/>
+      <c r="AAY2" s="0"/>
+      <c r="AAZ2" s="0"/>
+      <c r="ABA2" s="0"/>
+      <c r="ABB2" s="0"/>
+      <c r="ABC2" s="0"/>
+      <c r="ABD2" s="0"/>
+      <c r="ABE2" s="0"/>
+      <c r="ABF2" s="0"/>
+      <c r="ABG2" s="0"/>
+      <c r="ABH2" s="0"/>
+      <c r="ABI2" s="0"/>
+      <c r="ABJ2" s="0"/>
+      <c r="ABK2" s="0"/>
+      <c r="ABL2" s="0"/>
+      <c r="ABM2" s="0"/>
+      <c r="ABN2" s="0"/>
+      <c r="ABO2" s="0"/>
+      <c r="ABP2" s="0"/>
+      <c r="ABQ2" s="0"/>
+      <c r="ABR2" s="0"/>
+      <c r="ABS2" s="0"/>
+      <c r="ABT2" s="0"/>
+      <c r="ABU2" s="0"/>
+      <c r="ABV2" s="0"/>
+      <c r="ABW2" s="0"/>
+      <c r="ABX2" s="0"/>
+      <c r="ABY2" s="0"/>
+      <c r="ABZ2" s="0"/>
+      <c r="ACA2" s="0"/>
+      <c r="ACB2" s="0"/>
+      <c r="ACC2" s="0"/>
+      <c r="ACD2" s="0"/>
+      <c r="ACE2" s="0"/>
+      <c r="ACF2" s="0"/>
+      <c r="ACG2" s="0"/>
+      <c r="ACH2" s="0"/>
+      <c r="ACI2" s="0"/>
+      <c r="ACJ2" s="0"/>
+      <c r="ACK2" s="0"/>
+      <c r="ACL2" s="0"/>
+      <c r="ACM2" s="0"/>
+      <c r="ACN2" s="0"/>
+      <c r="ACO2" s="0"/>
+      <c r="ACP2" s="0"/>
+      <c r="ACQ2" s="0"/>
+      <c r="ACR2" s="0"/>
+      <c r="ACS2" s="0"/>
+      <c r="ACT2" s="0"/>
+      <c r="ACU2" s="0"/>
+      <c r="ACV2" s="0"/>
+      <c r="ACW2" s="0"/>
+      <c r="ACX2" s="0"/>
+      <c r="ACY2" s="0"/>
+      <c r="ACZ2" s="0"/>
+      <c r="ADA2" s="0"/>
+      <c r="ADB2" s="0"/>
+      <c r="ADC2" s="0"/>
+      <c r="ADD2" s="0"/>
+      <c r="ADE2" s="0"/>
+      <c r="ADF2" s="0"/>
+      <c r="ADG2" s="0"/>
+      <c r="ADH2" s="0"/>
+      <c r="ADI2" s="0"/>
+      <c r="ADJ2" s="0"/>
+      <c r="ADK2" s="0"/>
+      <c r="ADL2" s="0"/>
+      <c r="ADM2" s="0"/>
+      <c r="ADN2" s="0"/>
+      <c r="ADO2" s="0"/>
+      <c r="ADP2" s="0"/>
+      <c r="ADQ2" s="0"/>
+      <c r="ADR2" s="0"/>
+      <c r="ADS2" s="0"/>
+      <c r="ADT2" s="0"/>
+      <c r="ADU2" s="0"/>
+      <c r="ADV2" s="0"/>
+      <c r="ADW2" s="0"/>
+      <c r="ADX2" s="0"/>
+      <c r="ADY2" s="0"/>
+      <c r="ADZ2" s="0"/>
+      <c r="AEA2" s="0"/>
+      <c r="AEB2" s="0"/>
+      <c r="AEC2" s="0"/>
+      <c r="AED2" s="0"/>
+      <c r="AEE2" s="0"/>
+      <c r="AEF2" s="0"/>
+      <c r="AEG2" s="0"/>
+      <c r="AEH2" s="0"/>
+      <c r="AEI2" s="0"/>
+      <c r="AEJ2" s="0"/>
+      <c r="AEK2" s="0"/>
+      <c r="AEL2" s="0"/>
+      <c r="AEM2" s="0"/>
+      <c r="AEN2" s="0"/>
+      <c r="AEO2" s="0"/>
+      <c r="AEP2" s="0"/>
+      <c r="AEQ2" s="0"/>
+      <c r="AER2" s="0"/>
+      <c r="AES2" s="0"/>
+      <c r="AET2" s="0"/>
+      <c r="AEU2" s="0"/>
+      <c r="AEV2" s="0"/>
+      <c r="AEW2" s="0"/>
+      <c r="AEX2" s="0"/>
+      <c r="AEY2" s="0"/>
+      <c r="AEZ2" s="0"/>
+      <c r="AFA2" s="0"/>
+      <c r="AFB2" s="0"/>
+      <c r="AFC2" s="0"/>
+      <c r="AFD2" s="0"/>
+      <c r="AFE2" s="0"/>
+      <c r="AFF2" s="0"/>
+      <c r="AFG2" s="0"/>
+      <c r="AFH2" s="0"/>
+      <c r="AFI2" s="0"/>
+      <c r="AFJ2" s="0"/>
+      <c r="AFK2" s="0"/>
+      <c r="AFL2" s="0"/>
+      <c r="AFM2" s="0"/>
+      <c r="AFN2" s="0"/>
+      <c r="AFO2" s="0"/>
+      <c r="AFP2" s="0"/>
+      <c r="AFQ2" s="0"/>
+      <c r="AFR2" s="0"/>
+      <c r="AFS2" s="0"/>
+      <c r="AFT2" s="0"/>
+      <c r="AFU2" s="0"/>
+      <c r="AFV2" s="0"/>
+      <c r="AFW2" s="0"/>
+      <c r="AFX2" s="0"/>
+      <c r="AFY2" s="0"/>
+      <c r="AFZ2" s="0"/>
+      <c r="AGA2" s="0"/>
+      <c r="AGB2" s="0"/>
+      <c r="AGC2" s="0"/>
+      <c r="AGD2" s="0"/>
+      <c r="AGE2" s="0"/>
+      <c r="AGF2" s="0"/>
+      <c r="AGG2" s="0"/>
+      <c r="AGH2" s="0"/>
+      <c r="AGI2" s="0"/>
+      <c r="AGJ2" s="0"/>
+      <c r="AGK2" s="0"/>
+      <c r="AGL2" s="0"/>
+      <c r="AGM2" s="0"/>
+      <c r="AGN2" s="0"/>
+      <c r="AGO2" s="0"/>
+      <c r="AGP2" s="0"/>
+      <c r="AGQ2" s="0"/>
+      <c r="AGR2" s="0"/>
+      <c r="AGS2" s="0"/>
+      <c r="AGT2" s="0"/>
+      <c r="AGU2" s="0"/>
+      <c r="AGV2" s="0"/>
+      <c r="AGW2" s="0"/>
+      <c r="AGX2" s="0"/>
+      <c r="AGY2" s="0"/>
+      <c r="AGZ2" s="0"/>
+      <c r="AHA2" s="0"/>
+      <c r="AHB2" s="0"/>
+      <c r="AHC2" s="0"/>
+      <c r="AHD2" s="0"/>
+      <c r="AHE2" s="0"/>
+      <c r="AHF2" s="0"/>
+      <c r="AHG2" s="0"/>
+      <c r="AHH2" s="0"/>
+      <c r="AHI2" s="0"/>
+      <c r="AHJ2" s="0"/>
+      <c r="AHK2" s="0"/>
+      <c r="AHL2" s="0"/>
+      <c r="AHM2" s="0"/>
+      <c r="AHN2" s="0"/>
+      <c r="AHO2" s="0"/>
+      <c r="AHP2" s="0"/>
+      <c r="AHQ2" s="0"/>
+      <c r="AHR2" s="0"/>
+      <c r="AHS2" s="0"/>
+      <c r="AHT2" s="0"/>
+      <c r="AHU2" s="0"/>
+      <c r="AHV2" s="0"/>
+      <c r="AHW2" s="0"/>
+      <c r="AHX2" s="0"/>
+      <c r="AHY2" s="0"/>
+      <c r="AHZ2" s="0"/>
+      <c r="AIA2" s="0"/>
+      <c r="AIB2" s="0"/>
+      <c r="AIC2" s="0"/>
+      <c r="AID2" s="0"/>
+      <c r="AIE2" s="0"/>
+      <c r="AIF2" s="0"/>
+      <c r="AIG2" s="0"/>
+      <c r="AIH2" s="0"/>
+      <c r="AII2" s="0"/>
+      <c r="AIJ2" s="0"/>
+      <c r="AIK2" s="0"/>
+      <c r="AIL2" s="0"/>
+      <c r="AIM2" s="0"/>
+      <c r="AIN2" s="0"/>
+      <c r="AIO2" s="0"/>
+      <c r="AIP2" s="0"/>
+      <c r="AIQ2" s="0"/>
+      <c r="AIR2" s="0"/>
+      <c r="AIS2" s="0"/>
+      <c r="AIT2" s="0"/>
+      <c r="AIU2" s="0"/>
+      <c r="AIV2" s="0"/>
+      <c r="AIW2" s="0"/>
+      <c r="AIX2" s="0"/>
+      <c r="AIY2" s="0"/>
+      <c r="AIZ2" s="0"/>
+      <c r="AJA2" s="0"/>
+      <c r="AJB2" s="0"/>
+      <c r="AJC2" s="0"/>
+      <c r="AJD2" s="0"/>
+      <c r="AJE2" s="0"/>
+      <c r="AJF2" s="0"/>
+      <c r="AJG2" s="0"/>
+      <c r="AJH2" s="0"/>
+      <c r="AJI2" s="0"/>
+      <c r="AJJ2" s="0"/>
+      <c r="AJK2" s="0"/>
+      <c r="AJL2" s="0"/>
+      <c r="AJM2" s="0"/>
+      <c r="AJN2" s="0"/>
+      <c r="AJO2" s="0"/>
+      <c r="AJP2" s="0"/>
+      <c r="AJQ2" s="0"/>
+      <c r="AJR2" s="0"/>
+      <c r="AJS2" s="0"/>
+      <c r="AJT2" s="0"/>
+      <c r="AJU2" s="0"/>
+      <c r="AJV2" s="0"/>
+      <c r="AJW2" s="0"/>
+      <c r="AJX2" s="0"/>
+      <c r="AJY2" s="0"/>
+      <c r="AJZ2" s="0"/>
+      <c r="AKA2" s="0"/>
+      <c r="AKB2" s="0"/>
+      <c r="AKC2" s="0"/>
+      <c r="AKD2" s="0"/>
+      <c r="AKE2" s="0"/>
+      <c r="AKF2" s="0"/>
+      <c r="AKG2" s="0"/>
+      <c r="AKH2" s="0"/>
+      <c r="AKI2" s="0"/>
+      <c r="AKJ2" s="0"/>
+      <c r="AKK2" s="0"/>
+      <c r="AKL2" s="0"/>
+      <c r="AKM2" s="0"/>
+      <c r="AKN2" s="0"/>
+      <c r="AKO2" s="0"/>
+      <c r="AKP2" s="0"/>
+      <c r="AKQ2" s="0"/>
+      <c r="AKR2" s="0"/>
+      <c r="AKS2" s="0"/>
+      <c r="AKT2" s="0"/>
+      <c r="AKU2" s="0"/>
+      <c r="AKV2" s="0"/>
+      <c r="AKW2" s="0"/>
+      <c r="AKX2" s="0"/>
+      <c r="AKY2" s="0"/>
+      <c r="AKZ2" s="0"/>
+      <c r="ALA2" s="0"/>
+      <c r="ALB2" s="0"/>
+      <c r="ALC2" s="0"/>
+      <c r="ALD2" s="0"/>
+      <c r="ALE2" s="0"/>
+      <c r="ALF2" s="0"/>
+      <c r="ALG2" s="0"/>
+      <c r="ALH2" s="0"/>
+      <c r="ALI2" s="0"/>
+      <c r="ALJ2" s="0"/>
+      <c r="ALK2" s="0"/>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -30862,7 +31995,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -31073,7 +32206,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
@@ -32258,10 +33391,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -32273,10 +33406,11 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.0890688259109"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.3684210526316"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="87.0890688259109"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.54251012145749"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
         <v>404</v>
       </c>
@@ -32298,363 +33432,377 @@
       <c r="G1" s="38" t="s">
         <v>410</v>
       </c>
+      <c r="H1" s="39" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39" t="s">
-        <v>411</v>
-      </c>
-      <c r="C2" s="39" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40" t="s">
         <v>412</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>413</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>414</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="E2" s="40" t="s">
         <v>415</v>
       </c>
-      <c r="G2" s="39"/>
+      <c r="F2" s="40" t="s">
+        <v>416</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="66.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="n">
+      <c r="A3" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>417</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>419</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" customFormat="false" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
-        <v>418</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>419</v>
-      </c>
-      <c r="E4" s="40" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="42" t="s">
         <v>420</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="D4" s="42" t="s">
         <v>421</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="E4" s="42" t="s">
+        <v>422</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>423</v>
+      </c>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40" t="s">
-        <v>422</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>423</v>
-      </c>
-      <c r="E5" s="40" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="42" t="s">
         <v>424</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="41"/>
+      <c r="D5" s="42" t="s">
+        <v>425</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>426</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40" t="s">
-        <v>425</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>426</v>
-      </c>
-      <c r="E6" s="40" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="42" t="s">
         <v>427</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="D6" s="42" t="s">
+        <v>428</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>429</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39" t="s">
-        <v>428</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>429</v>
-      </c>
-      <c r="E7" s="39" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40" t="s">
         <v>430</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="39" t="s">
+      <c r="D7" s="40" t="s">
         <v>431</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>432</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="40" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39" t="s">
-        <v>432</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>429</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>433</v>
-      </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="39"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40" t="s">
+        <v>434</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>431</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>435</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="40"/>
     </row>
-    <row r="9" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39" t="s">
-        <v>434</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>435</v>
-      </c>
-      <c r="E9" s="39" t="s">
+    <row r="9" customFormat="false" ht="176.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40" t="s">
         <v>436</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="D9" s="40" t="s">
+        <v>437</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>438</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="34" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="39" t="s">
-        <v>437</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>438</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>439</v>
-      </c>
-      <c r="F10" s="39" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="40" t="s">
         <v>440</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="D10" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>443</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="0" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="n">
+      <c r="A11" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>441</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>442</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>443</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>444</v>
-      </c>
-      <c r="G11" s="39"/>
+      <c r="C11" s="40" t="s">
+        <v>445</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>447</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>448</v>
+      </c>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39" t="s">
-        <v>445</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>446</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>448</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40" t="s">
+        <v>449</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>450</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>451</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>452</v>
+      </c>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39" t="s">
-        <v>449</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>450</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>451</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40" t="s">
+        <v>453</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>454</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>455</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39" t="s">
-        <v>452</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>453</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>454</v>
-      </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40" t="s">
+        <v>456</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>457</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>458</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39" t="s">
-        <v>455</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>456</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>457</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40" t="s">
+        <v>459</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>460</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>461</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39" t="s">
-        <v>458</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>459</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>460</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40" t="s">
+        <v>462</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>463</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>464</v>
+      </c>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39" t="s">
-        <v>461</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>462</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>463</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40" t="s">
+        <v>465</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="41" t="s">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>464</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>465</v>
-      </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+      <c r="D18" s="40" t="s">
+        <v>468</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39" t="s">
-        <v>466</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>467</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>468</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>471</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>472</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39" t="s">
-        <v>470</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>471</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>472</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>473</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40" t="s">
+        <v>474</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>475</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>476</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>477</v>
+      </c>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39" t="s">
-        <v>474</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>475</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>476</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>477</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40" t="s">
+        <v>478</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>479</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>480</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>481</v>
+      </c>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="234" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39" t="s">
-        <v>478</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>479</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>480</v>
-      </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40" t="s">
+        <v>482</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>483</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>484</v>
+      </c>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39" t="s">
-        <v>481</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40" t="s">
+        <v>485</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="F4:F8"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="B12:B18"/>
@@ -32698,7 +33846,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32706,7 +33854,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32714,7 +33862,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32722,7 +33870,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32730,7 +33878,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32738,7 +33886,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32746,7 +33894,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32754,7 +33902,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32762,7 +33910,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32770,7 +33918,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32778,7 +33926,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32786,7 +33934,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32794,7 +33942,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32802,7 +33950,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32810,7 +33958,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>